<commit_message>
Figured out how to get parallelism to happen... innner loop has to take enough time.
</commit_message>
<xml_diff>
--- a/src/Simulation/Native/stats.xlsx
+++ b/src/Simulation/Native/stats.xlsx
@@ -5,20 +5,21 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\depot\Git\msr-quarc\wecker\QDK\integer-factorization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\depot\Git\qsharp-runtime\src\Simulation\Native\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55AB4B40-2441-414B-8B4E-09D1F243A236}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D16DA60-4BCF-47FD-9E55-2B202171A7C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13872" yWindow="8256" windowWidth="16080" windowHeight="10788" activeTab="1" xr2:uid="{5FEEEFE3-C5E9-4691-A26D-4009EEFDD3E5}"/>
+    <workbookView xWindow="624" yWindow="7932" windowWidth="16080" windowHeight="10788" activeTab="2" xr2:uid="{5FEEEFE3-C5E9-4691-A26D-4009EEFDD3E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
     <sheet name="Runs" sheetId="2" r:id="rId2"/>
+    <sheet name="Simple Test" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="30" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="55">
   <si>
     <t>Time (s)</t>
   </si>
@@ -254,6 +255,15 @@
   <si>
     <t>WU</t>
   </si>
+  <si>
+    <t>WU2</t>
+  </si>
+  <si>
+    <t>Benchmark speed up factors  (8e2,2e6):</t>
+  </si>
+  <si>
+    <t>Benchmark speed up factors  (8e7,2e1):</t>
+  </si>
 </sst>
 </file>
 
@@ -365,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -456,74 +466,13 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="58">
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
+  <dxfs count="19">
     <dxf>
       <alignment horizontal="center"/>
     </dxf>
@@ -580,60 +529,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3248,7 +3143,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CF1768AF-73FC-4A05-B410-0579B3B8096E}" name="PivotTable1" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Fusion, Thrds" colHeaderCaption=" ">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CF1768AF-73FC-4A05-B410-0579B3B8096E}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Fusion, Thrds" colHeaderCaption=" ">
   <location ref="K2:T29" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisCol" showAll="0">
@@ -3416,36 +3311,36 @@
     <dataField name="kGpS " fld="7" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
   <formats count="19">
-    <format dxfId="38">
+    <format dxfId="18">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="39">
+    <format dxfId="17">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="40">
+    <format dxfId="16">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="41">
+    <format dxfId="15">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="42">
+    <format dxfId="14">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="43">
+    <format dxfId="13">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="44">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="45">
+    <format dxfId="11">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -3455,7 +3350,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="46">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -3465,7 +3360,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="47">
+    <format dxfId="9">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -3475,29 +3370,29 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="27">
+    <format dxfId="8">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="26">
+    <format dxfId="7">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="25">
+    <format dxfId="6">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="24">
+    <format dxfId="5">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="23">
+    <format dxfId="4">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="22">
+    <format dxfId="3">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="21">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -3507,7 +3402,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="20">
+    <format dxfId="1">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -3517,7 +3412,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="19">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -4870,7 +4765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB803F0-8526-4AD8-A3BB-F38B006D6766}">
   <dimension ref="A1:W193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O42" sqref="O42"/>
     </sheetView>
   </sheetViews>
@@ -10839,4 +10734,316 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5345642-87ED-41EA-A14F-EAA5E00ADC38}">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="4" width="8.88671875" style="31"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="31">
+        <v>1</v>
+      </c>
+      <c r="B3" s="31">
+        <v>1</v>
+      </c>
+      <c r="C3" s="31">
+        <v>1</v>
+      </c>
+      <c r="D3" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="31">
+        <v>2</v>
+      </c>
+      <c r="B4" s="31">
+        <v>1.94</v>
+      </c>
+      <c r="C4" s="31">
+        <v>1.07</v>
+      </c>
+      <c r="D4" s="31">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="31">
+        <v>3</v>
+      </c>
+      <c r="B5" s="31">
+        <v>2.38</v>
+      </c>
+      <c r="C5" s="31">
+        <v>1.57</v>
+      </c>
+      <c r="D5" s="31">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="31">
+        <v>4</v>
+      </c>
+      <c r="B6" s="31">
+        <v>2.58</v>
+      </c>
+      <c r="C6" s="31">
+        <v>1.96</v>
+      </c>
+      <c r="D6" s="31">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="31">
+        <v>5</v>
+      </c>
+      <c r="B7" s="31">
+        <v>3.27</v>
+      </c>
+      <c r="C7" s="31">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="D7" s="31">
+        <v>1.54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="31">
+        <v>6</v>
+      </c>
+      <c r="B8" s="31">
+        <v>3.61</v>
+      </c>
+      <c r="C8" s="31">
+        <v>2.66</v>
+      </c>
+      <c r="D8" s="31">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="31">
+        <v>7</v>
+      </c>
+      <c r="B9" s="31">
+        <v>3.92</v>
+      </c>
+      <c r="C9" s="31">
+        <v>2.95</v>
+      </c>
+      <c r="D9" s="31">
+        <v>2.0699999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="31">
+        <v>8</v>
+      </c>
+      <c r="B10" s="31">
+        <v>4.42</v>
+      </c>
+      <c r="C10" s="31">
+        <v>3.19</v>
+      </c>
+      <c r="D10" s="31">
+        <v>2.34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="31">
+        <v>1</v>
+      </c>
+      <c r="B14" s="31">
+        <v>1</v>
+      </c>
+      <c r="C14" s="31">
+        <v>1</v>
+      </c>
+      <c r="D14" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="31">
+        <v>2</v>
+      </c>
+      <c r="B15" s="31">
+        <v>2.04</v>
+      </c>
+      <c r="C15" s="31">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="D15" s="31">
+        <v>1.93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="31">
+        <v>3</v>
+      </c>
+      <c r="B16" s="31">
+        <v>3.03</v>
+      </c>
+      <c r="C16" s="31">
+        <v>3.03</v>
+      </c>
+      <c r="D16" s="31">
+        <v>2.83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="31">
+        <v>4</v>
+      </c>
+      <c r="B17" s="31">
+        <v>4.05</v>
+      </c>
+      <c r="C17" s="31">
+        <v>4.03</v>
+      </c>
+      <c r="D17" s="31">
+        <v>3.74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="31">
+        <v>5</v>
+      </c>
+      <c r="B18" s="31">
+        <v>5.04</v>
+      </c>
+      <c r="C18" s="31">
+        <v>5.04</v>
+      </c>
+      <c r="D18" s="31">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="31">
+        <v>6</v>
+      </c>
+      <c r="B19" s="31">
+        <v>6.03</v>
+      </c>
+      <c r="C19" s="31">
+        <v>6.01</v>
+      </c>
+      <c r="D19" s="31">
+        <v>5.61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="31">
+        <v>7</v>
+      </c>
+      <c r="B20" s="31">
+        <v>6.99</v>
+      </c>
+      <c r="C20" s="31">
+        <v>6.96</v>
+      </c>
+      <c r="D20" s="31">
+        <v>6.54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="31">
+        <v>8</v>
+      </c>
+      <c r="B21" s="31">
+        <v>7.79</v>
+      </c>
+      <c r="C21" s="31">
+        <v>7.85</v>
+      </c>
+      <c r="D21" s="31">
+        <v>7.47</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B3:D10">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="num" val="8"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:D21">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="num" val="8"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Doing full stat run
</commit_message>
<xml_diff>
--- a/src/Simulation/Native/stats.xlsx
+++ b/src/Simulation/Native/stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\depot\Git\qsharp-runtime\src\Simulation\Native\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D16DA60-4BCF-47FD-9E55-2B202171A7C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FB45A0-6C29-4A75-A120-69550F28B23F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="624" yWindow="7932" windowWidth="16080" windowHeight="10788" activeTab="2" xr2:uid="{5FEEEFE3-C5E9-4691-A26D-4009EEFDD3E5}"/>
+    <workbookView xWindow="624" yWindow="7932" windowWidth="16080" windowHeight="10788" activeTab="1" xr2:uid="{5FEEEFE3-C5E9-4691-A26D-4009EEFDD3E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="56">
   <si>
     <t>Time (s)</t>
   </si>
@@ -263,6 +263,9 @@
   </si>
   <si>
     <t>Benchmark speed up factors  (8e7,2e1):</t>
+  </si>
+  <si>
+    <t>xxxx</t>
   </si>
 </sst>
 </file>
@@ -4765,8 +4768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB803F0-8526-4AD8-A3BB-F38B006D6766}">
   <dimension ref="A1:W193"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O42" sqref="O42"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4884,7 +4887,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="27">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K2" s="32" t="s">
         <v>41</v>
@@ -5031,7 +5034,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="27">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K5" s="23" t="s">
         <v>43</v>
@@ -5072,7 +5075,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="27">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="K6" s="24">
         <v>1</v>
@@ -5131,7 +5134,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="27">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="K7" s="24">
         <v>2</v>
@@ -5190,7 +5193,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="27">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="K8" s="24">
         <v>3</v>
@@ -5249,7 +5252,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="27">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K9" s="24">
         <v>4</v>
@@ -5308,7 +5311,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="27">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="K10" s="23" t="s">
         <v>44</v>
@@ -5349,7 +5352,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="27">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K11" s="24">
         <v>1</v>
@@ -5408,7 +5411,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="27">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="K12" s="24">
         <v>2</v>
@@ -5467,7 +5470,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="27">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="K13" s="24">
         <v>3</v>
@@ -5526,7 +5529,7 @@
         <v>0.95</v>
       </c>
       <c r="H14" s="27">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K14" s="24">
         <v>4</v>
@@ -5685,7 +5688,7 @@
         <v>0.95</v>
       </c>
       <c r="H17" s="27">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="K17" s="24">
         <v>2</v>
@@ -5744,7 +5747,7 @@
         <v>0.95</v>
       </c>
       <c r="H18" s="27">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K18" s="24">
         <v>3</v>
@@ -5803,7 +5806,7 @@
         <v>0.95</v>
       </c>
       <c r="H19" s="27">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="K19" s="24">
         <v>4</v>
@@ -5862,7 +5865,7 @@
         <v>0.95</v>
       </c>
       <c r="H20" s="27">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="K20" s="23" t="s">
         <v>46</v>
@@ -5903,7 +5906,7 @@
         <v>0.95</v>
       </c>
       <c r="H21" s="27">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="K21" s="24">
         <v>1</v>
@@ -5962,7 +5965,7 @@
         <v>0.95</v>
       </c>
       <c r="H22" s="27">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="K22" s="24">
         <v>2</v>
@@ -6021,7 +6024,7 @@
         <v>0.95</v>
       </c>
       <c r="H23" s="27">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K23" s="24">
         <v>3</v>
@@ -6139,7 +6142,7 @@
         <v>0.95</v>
       </c>
       <c r="H25" s="27">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="K25" s="23" t="s">
         <v>47</v>
@@ -6239,7 +6242,7 @@
         <v>0</v>
       </c>
       <c r="H27" s="27">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="K27" s="24">
         <v>2</v>
@@ -6298,7 +6301,7 @@
         <v>0</v>
       </c>
       <c r="H28" s="27">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K28" s="24">
         <v>3</v>
@@ -6357,7 +6360,7 @@
         <v>0</v>
       </c>
       <c r="H29" s="27">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K29" s="24">
         <v>4</v>
@@ -6416,7 +6419,7 @@
         <v>0</v>
       </c>
       <c r="H30" s="27">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.3">
@@ -6442,7 +6445,7 @@
         <v>0</v>
       </c>
       <c r="H31" s="27">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.3">
@@ -6468,7 +6471,7 @@
         <v>0</v>
       </c>
       <c r="H32" s="27">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -6494,7 +6497,7 @@
         <v>0</v>
       </c>
       <c r="H33" s="27">
-        <v>66</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -6520,7 +6523,7 @@
         <v>0</v>
       </c>
       <c r="H34" s="27">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -6546,7 +6549,7 @@
         <v>0</v>
       </c>
       <c r="H35" s="27">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -6572,7 +6575,7 @@
         <v>0</v>
       </c>
       <c r="H36" s="27">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -6598,7 +6601,7 @@
         <v>0</v>
       </c>
       <c r="H37" s="27">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -6624,7 +6627,7 @@
         <v>0</v>
       </c>
       <c r="H38" s="28">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -6650,7 +6653,7 @@
         <v>0</v>
       </c>
       <c r="H39" s="28">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
@@ -6676,7 +6679,7 @@
         <v>0</v>
       </c>
       <c r="H40" s="28">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -6702,7 +6705,7 @@
         <v>0</v>
       </c>
       <c r="H41" s="28">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -7274,7 +7277,7 @@
         <v>0</v>
       </c>
       <c r="H63" s="27">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
@@ -7300,7 +7303,7 @@
         <v>0</v>
       </c>
       <c r="H64" s="27">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
@@ -7352,7 +7355,7 @@
         <v>0</v>
       </c>
       <c r="H66" s="27">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
@@ -7378,7 +7381,7 @@
         <v>0</v>
       </c>
       <c r="H67" s="27">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
@@ -7430,7 +7433,7 @@
         <v>0</v>
       </c>
       <c r="H69" s="27">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
@@ -7456,7 +7459,7 @@
         <v>0</v>
       </c>
       <c r="H70" s="27">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
@@ -7508,7 +7511,7 @@
         <v>0</v>
       </c>
       <c r="H72" s="27">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
@@ -7534,7 +7537,7 @@
         <v>0</v>
       </c>
       <c r="H73" s="27">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
@@ -7560,7 +7563,7 @@
         <v>0.95</v>
       </c>
       <c r="H74" s="27">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
@@ -7586,7 +7589,7 @@
         <v>0.95</v>
       </c>
       <c r="H75" s="27">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
@@ -7612,7 +7615,7 @@
         <v>0.95</v>
       </c>
       <c r="H76" s="27">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
@@ -7664,7 +7667,7 @@
         <v>0.95</v>
       </c>
       <c r="H78" s="27">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
@@ -7690,7 +7693,7 @@
         <v>0.95</v>
       </c>
       <c r="H79" s="27">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
@@ -7742,7 +7745,7 @@
         <v>0.95</v>
       </c>
       <c r="H81" s="27">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
@@ -7768,7 +7771,7 @@
         <v>0.95</v>
       </c>
       <c r="H82" s="27">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
@@ -7794,7 +7797,7 @@
         <v>0.95</v>
       </c>
       <c r="H83" s="27">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
@@ -7820,7 +7823,7 @@
         <v>0.95</v>
       </c>
       <c r="H84" s="27">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
@@ -7846,7 +7849,7 @@
         <v>0.95</v>
       </c>
       <c r="H85" s="27">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
@@ -7950,7 +7953,7 @@
         <v>0</v>
       </c>
       <c r="H89" s="27">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
@@ -7976,7 +7979,7 @@
         <v>0</v>
       </c>
       <c r="H90" s="27">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
@@ -8028,7 +8031,7 @@
         <v>0</v>
       </c>
       <c r="H92" s="27">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
@@ -8054,7 +8057,7 @@
         <v>0</v>
       </c>
       <c r="H93" s="27">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
@@ -8080,7 +8083,7 @@
         <v>0</v>
       </c>
       <c r="H94" s="28">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
@@ -8106,7 +8109,7 @@
         <v>0</v>
       </c>
       <c r="H95" s="27">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
@@ -8132,10 +8135,10 @@
         <v>0</v>
       </c>
       <c r="H96" s="27">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="25" t="s">
         <v>50</v>
       </c>
@@ -8158,10 +8161,10 @@
         <v>0</v>
       </c>
       <c r="H97" s="27">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="25" t="s">
         <v>50</v>
       </c>
@@ -8186,8 +8189,11 @@
       <c r="H98" s="28">
         <v>14</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I98" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="25" t="s">
         <v>50</v>
       </c>
@@ -8213,7 +8219,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="25" t="s">
         <v>50</v>
       </c>
@@ -8239,7 +8245,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="25" t="s">
         <v>50</v>
       </c>
@@ -8265,7 +8271,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="25" t="s">
         <v>50</v>
       </c>
@@ -8291,7 +8297,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="25" t="s">
         <v>50</v>
       </c>
@@ -8317,7 +8323,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="25" t="s">
         <v>50</v>
       </c>
@@ -8343,7 +8349,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="25" t="s">
         <v>50</v>
       </c>
@@ -8369,7 +8375,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="25" t="s">
         <v>50</v>
       </c>
@@ -8395,7 +8401,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" s="25" t="s">
         <v>50</v>
       </c>
@@ -8421,7 +8427,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" s="25" t="s">
         <v>50</v>
       </c>
@@ -8447,7 +8453,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" s="25" t="s">
         <v>50</v>
       </c>
@@ -8473,7 +8479,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" s="25" t="s">
         <v>50</v>
       </c>
@@ -8499,7 +8505,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="25" t="s">
         <v>50</v>
       </c>
@@ -8525,7 +8531,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" s="25" t="s">
         <v>50</v>
       </c>
@@ -10740,8 +10746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5345642-87ED-41EA-A14F-EAA5E00ADC38}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Going to try the old openMP code...
</commit_message>
<xml_diff>
--- a/src/Simulation/Native/stats.xlsx
+++ b/src/Simulation/Native/stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\depot\Git\qsharp-runtime\src\Simulation\Native\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129376EA-A830-4803-B7E5-2EBC9F3DABE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F18F7BB-C721-4F04-A7C3-AB7492191EBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13764" yWindow="8628" windowWidth="16080" windowHeight="10788" activeTab="1" xr2:uid="{5FEEEFE3-C5E9-4691-A26D-4009EEFDD3E5}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="30" r:id="rId4"/>
+    <pivotCache cacheId="12" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="57">
   <si>
     <t>Time (s)</t>
   </si>
@@ -267,6 +267,9 @@
   <si>
     <t>Scale factor</t>
   </si>
+  <si>
+    <t>W15tp</t>
+  </si>
 </sst>
 </file>
 
@@ -475,64 +478,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="95">
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
+  <dxfs count="76">
     <dxf>
       <alignment horizontal="center"/>
     </dxf>
@@ -775,16 +721,17 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Dave Wecker" refreshedDate="43971.678834722225" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="238" xr:uid="{22FAA616-9F74-4145-9671-E5F5B83F2D90}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Dave Wecker" refreshedDate="43973.651789467593" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="304" xr:uid="{22FAA616-9F74-4145-9671-E5F5B83F2D90}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:H1048576" sheet="Runs"/>
   </cacheSource>
   <cacheFields count="8">
     <cacheField name="Env" numFmtId="0">
-      <sharedItems containsBlank="1" count="6">
+      <sharedItems containsBlank="1" count="7">
         <s v="W15"/>
         <s v="W15_WSL"/>
         <s v="WU"/>
+        <s v="W15tp"/>
         <m/>
         <s v="W1" u="1"/>
         <s v="WU_WSL" u="1"/>
@@ -828,7 +775,7 @@
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0" maxValue="0.95"/>
     </cacheField>
     <cacheField name="kGpS" numFmtId="1">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="5" maxValue="99"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="4" maxValue="99"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -840,7 +787,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="238">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="304">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -3093,6 +3040,756 @@
   </r>
   <r>
     <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="6"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="8"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="8"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="11"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="14"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="17"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="17"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="14"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="11"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="1"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1.05"/>
+    <n v="1"/>
+    <n v="0.95"/>
+    <n v="7"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1.05"/>
+    <n v="1"/>
+    <n v="0.95"/>
+    <n v="9"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1.05"/>
+    <n v="1"/>
+    <n v="0.95"/>
+    <n v="9"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1.05"/>
+    <n v="1"/>
+    <n v="0.95"/>
+    <n v="12"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1.05"/>
+    <n v="1"/>
+    <n v="0.95"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1.05"/>
+    <n v="1"/>
+    <n v="0.95"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1.05"/>
+    <n v="1"/>
+    <n v="0.95"/>
+    <n v="16"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1.05"/>
+    <n v="1"/>
+    <n v="0.95"/>
+    <n v="18"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1.05"/>
+    <n v="1"/>
+    <n v="0.95"/>
+    <n v="18"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="1.05"/>
+    <n v="1"/>
+    <n v="0.95"/>
+    <n v="14"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="1.05"/>
+    <n v="1"/>
+    <n v="0.95"/>
+    <n v="16"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="1.05"/>
+    <n v="1"/>
+    <n v="0.95"/>
+    <n v="14"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="1.05"/>
+    <n v="1"/>
+    <n v="0.95"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="1.05"/>
+    <n v="1"/>
+    <n v="0.95"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="1.05"/>
+    <n v="1"/>
+    <n v="0.95"/>
+    <n v="10"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="3.04"/>
+    <n v="1.96"/>
+    <n v="0"/>
+    <n v="11"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="3.04"/>
+    <n v="1.96"/>
+    <n v="0"/>
+    <n v="16"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="3.04"/>
+    <n v="1.96"/>
+    <n v="0"/>
+    <n v="17"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="3.04"/>
+    <n v="1.96"/>
+    <n v="0"/>
+    <n v="20"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="3.04"/>
+    <n v="1.96"/>
+    <n v="0"/>
+    <n v="27"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="3.04"/>
+    <n v="1.96"/>
+    <n v="0"/>
+    <n v="29"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="3.04"/>
+    <n v="1.96"/>
+    <n v="0"/>
+    <n v="24"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="3.04"/>
+    <n v="1.96"/>
+    <n v="0"/>
+    <n v="32"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="3.04"/>
+    <n v="1.96"/>
+    <n v="0"/>
+    <n v="33"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="3.04"/>
+    <n v="1.96"/>
+    <n v="0"/>
+    <n v="25"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="3.04"/>
+    <n v="1.96"/>
+    <n v="0"/>
+    <n v="30"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="3.04"/>
+    <n v="1.96"/>
+    <n v="0"/>
+    <n v="34"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="3.04"/>
+    <n v="1.96"/>
+    <n v="0"/>
+    <n v="25"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="3.04"/>
+    <n v="1.96"/>
+    <n v="0"/>
+    <n v="30"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="3.04"/>
+    <n v="1.96"/>
+    <n v="0"/>
+    <n v="30"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="8"/>
+    <n v="3"/>
+    <n v="0"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="8"/>
+    <n v="3"/>
+    <n v="0"/>
+    <n v="27"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="8"/>
+    <n v="3"/>
+    <n v="0"/>
+    <n v="31"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="8"/>
+    <n v="3"/>
+    <n v="0"/>
+    <n v="25"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="8"/>
+    <n v="3"/>
+    <n v="0"/>
+    <n v="42"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="8"/>
+    <n v="3"/>
+    <n v="0"/>
+    <n v="47"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="8"/>
+    <n v="3"/>
+    <n v="0"/>
+    <n v="31"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="8"/>
+    <n v="3"/>
+    <n v="0"/>
+    <n v="51"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="8"/>
+    <n v="3"/>
+    <n v="0"/>
+    <n v="54"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="8"/>
+    <n v="3"/>
+    <n v="0"/>
+    <n v="32"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="8"/>
+    <n v="3"/>
+    <n v="0"/>
+    <n v="49"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="8"/>
+    <n v="3"/>
+    <n v="0"/>
+    <n v="54"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="3"/>
+    <n v="8"/>
+    <n v="3"/>
+    <n v="0"/>
+    <n v="32"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="3"/>
+    <n v="8"/>
+    <n v="3"/>
+    <n v="0"/>
+    <n v="49"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="3"/>
+    <n v="8"/>
+    <n v="3"/>
+    <n v="0"/>
+    <n v="53"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="13.7"/>
+    <n v="3.97"/>
+    <n v="0"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="13.7"/>
+    <n v="3.97"/>
+    <n v="0"/>
+    <n v="22"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="13.7"/>
+    <n v="3.97"/>
+    <n v="0"/>
+    <n v="24"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="13.7"/>
+    <n v="3.97"/>
+    <n v="0"/>
+    <n v="8"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="13.7"/>
+    <n v="3.97"/>
+    <n v="0"/>
+    <n v="28"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="13.7"/>
+    <n v="3.97"/>
+    <n v="0"/>
+    <n v="32"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="13.7"/>
+    <n v="3.97"/>
+    <n v="0"/>
+    <n v="11"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="13.7"/>
+    <n v="3.97"/>
+    <n v="0"/>
+    <n v="35"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="13.7"/>
+    <n v="3.97"/>
+    <n v="0"/>
+    <n v="38"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="13.7"/>
+    <n v="3.97"/>
+    <n v="0"/>
+    <n v="13"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="13.7"/>
+    <n v="3.97"/>
+    <n v="0"/>
+    <n v="37"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="13.7"/>
+    <n v="3.97"/>
+    <n v="0"/>
+    <n v="40"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="13.7"/>
+    <n v="3.97"/>
+    <n v="0"/>
+    <n v="15"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="13.7"/>
+    <n v="3.97"/>
+    <n v="0"/>
+    <n v="38"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="13.7"/>
+    <n v="3.97"/>
+    <n v="0"/>
+    <n v="41"/>
+  </r>
+  <r>
+    <x v="4"/>
     <x v="3"/>
     <x v="5"/>
     <x v="5"/>
@@ -3102,7 +3799,7 @@
     <m/>
   </r>
   <r>
-    <x v="3"/>
+    <x v="4"/>
     <x v="3"/>
     <x v="5"/>
     <x v="5"/>
@@ -3112,7 +3809,7 @@
     <m/>
   </r>
   <r>
-    <x v="3"/>
+    <x v="4"/>
     <x v="3"/>
     <x v="5"/>
     <x v="5"/>
@@ -3122,7 +3819,7 @@
     <m/>
   </r>
   <r>
-    <x v="3"/>
+    <x v="4"/>
     <x v="3"/>
     <x v="5"/>
     <x v="5"/>
@@ -3131,111 +3828,22 @@
     <m/>
     <m/>
   </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-    <x v="5"/>
-    <x v="5"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-    <x v="5"/>
-    <x v="5"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-    <x v="5"/>
-    <x v="5"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-    <x v="5"/>
-    <x v="5"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-    <x v="5"/>
-    <x v="5"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-    <x v="5"/>
-    <x v="5"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-    <x v="5"/>
-    <x v="5"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-    <x v="5"/>
-    <x v="5"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="3"/>
-    <x v="3"/>
-    <x v="5"/>
-    <x v="5"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CF1768AF-73FC-4A05-B410-0579B3B8096E}" name="PivotTable1" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Fusion, Thrds" colHeaderCaption=" ">
-  <location ref="J2:S34" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CF1768AF-73FC-4A05-B410-0579B3B8096E}" name="PivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Fusion, Thrds" colHeaderCaption=" ">
+  <location ref="J2:V34" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisCol" showAll="0">
-      <items count="7">
+      <items count="8">
         <item x="0"/>
         <item x="1"/>
-        <item h="1" x="3"/>
-        <item h="1" m="1" x="4"/>
-        <item m="1" x="5"/>
+        <item h="1" x="4"/>
+        <item h="1" m="1" x="5"/>
+        <item m="1" x="6"/>
         <item x="2"/>
+        <item x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -3373,7 +3981,7 @@
     <field x="1"/>
     <field x="0"/>
   </colFields>
-  <colItems count="9">
+  <colItems count="12">
     <i>
       <x v="1"/>
       <x/>
@@ -3383,6 +3991,9 @@
     </i>
     <i r="1">
       <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
     </i>
     <i>
       <x v="2"/>
@@ -3394,6 +4005,9 @@
     <i r="1">
       <x v="5"/>
     </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
     <i>
       <x v="3"/>
       <x/>
@@ -3404,41 +4018,44 @@
     <i r="1">
       <x v="5"/>
     </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
   </colItems>
   <dataFields count="1">
     <dataField name="kGpS " fld="7" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
   <formats count="19">
-    <format dxfId="94">
+    <format dxfId="75">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="93">
+    <format dxfId="74">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="92">
+    <format dxfId="73">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="91">
+    <format dxfId="72">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="90">
+    <format dxfId="71">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="89">
+    <format dxfId="70">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="88">
+    <format dxfId="69">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="87">
+    <format dxfId="68">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -3448,7 +4065,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="86">
+    <format dxfId="67">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -3458,7 +4075,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="85">
+    <format dxfId="66">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -3468,29 +4085,29 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="84">
+    <format dxfId="65">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="83">
+    <format dxfId="64">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="82">
+    <format dxfId="63">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="81">
+    <format dxfId="62">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="80">
+    <format dxfId="61">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="79">
+    <format dxfId="60">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="78">
+    <format dxfId="59">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -3500,7 +4117,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="77">
+    <format dxfId="58">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -3510,7 +4127,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="76">
+    <format dxfId="57">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -4861,10 +5478,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB803F0-8526-4AD8-A3BB-F38B006D6766}">
-  <dimension ref="A1:W238"/>
+  <dimension ref="A1:W304"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4875,14 +5492,14 @@
     <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.44140625" style="29" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4.109375" style="29" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.5546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.44140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.109375" style="29" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.5546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.44140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="4.109375" style="29" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.44140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.77734375" style="29" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="6.5546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.44140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.5546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.5546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.44140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.109375" style="29" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.5546875" style="29" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="4.109375" style="29" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="3.77734375" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="8.77734375" bestFit="1" customWidth="1"/>
@@ -4998,8 +5615,9 @@
       <c r="Q2" s="30"/>
       <c r="R2" s="30"/>
       <c r="S2" s="30"/>
-      <c r="U2"/>
-      <c r="V2"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="30"/>
+      <c r="V2" s="30"/>
       <c r="W2"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
@@ -5033,18 +5651,19 @@
       </c>
       <c r="L3" s="30"/>
       <c r="M3" s="30"/>
-      <c r="N3" s="30" t="s">
+      <c r="N3" s="30"/>
+      <c r="O3" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="O3" s="30"/>
       <c r="P3" s="30"/>
-      <c r="Q3" s="30" t="s">
+      <c r="Q3" s="30"/>
+      <c r="R3" s="30"/>
+      <c r="S3" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
-      <c r="U3"/>
-      <c r="V3"/>
+      <c r="T3" s="30"/>
+      <c r="U3" s="30"/>
+      <c r="V3" s="30"/>
       <c r="W3"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
@@ -5085,25 +5704,32 @@
         <v>51</v>
       </c>
       <c r="N4" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="O4" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="O4" s="30" t="s">
+      <c r="P4" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="P4" s="30" t="s">
+      <c r="Q4" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="Q4" s="30" t="s">
+      <c r="R4" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="S4" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="R4" s="30" t="s">
+      <c r="T4" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="S4" s="30" t="s">
+      <c r="U4" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="U4"/>
-      <c r="V4"/>
+      <c r="V4" s="30" t="s">
+        <v>56</v>
+      </c>
       <c r="W4"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
@@ -5143,8 +5769,9 @@
       <c r="Q5" s="30"/>
       <c r="R5" s="30"/>
       <c r="S5" s="30"/>
-      <c r="U5"/>
-      <c r="V5"/>
+      <c r="T5" s="30"/>
+      <c r="U5" s="30"/>
+      <c r="V5" s="30"/>
       <c r="W5"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
@@ -5185,25 +5812,32 @@
         <v>9</v>
       </c>
       <c r="N6" s="30">
+        <v>6</v>
+      </c>
+      <c r="O6" s="30">
         <v>28</v>
       </c>
-      <c r="O6" s="30">
+      <c r="P6" s="30">
         <v>34</v>
       </c>
-      <c r="P6" s="30">
+      <c r="Q6" s="30">
         <v>39</v>
       </c>
-      <c r="Q6" s="30">
+      <c r="R6" s="30">
+        <v>8</v>
+      </c>
+      <c r="S6" s="30">
         <v>32</v>
       </c>
-      <c r="R6" s="30">
+      <c r="T6" s="30">
         <v>34</v>
       </c>
-      <c r="S6" s="30">
+      <c r="U6" s="30">
         <v>39</v>
       </c>
-      <c r="U6"/>
-      <c r="V6"/>
+      <c r="V6" s="30">
+        <v>8</v>
+      </c>
       <c r="W6"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
@@ -5244,25 +5878,32 @@
         <v>16.5</v>
       </c>
       <c r="N7" s="30">
+        <v>11</v>
+      </c>
+      <c r="O7" s="30">
         <v>43</v>
       </c>
-      <c r="O7" s="30">
+      <c r="P7" s="30">
         <v>53</v>
       </c>
-      <c r="P7" s="30">
+      <c r="Q7" s="30">
         <v>57</v>
       </c>
-      <c r="Q7" s="30">
+      <c r="R7" s="30">
+        <v>14</v>
+      </c>
+      <c r="S7" s="30">
         <v>44</v>
       </c>
-      <c r="R7" s="30">
+      <c r="T7" s="30">
         <v>53</v>
       </c>
-      <c r="S7" s="30">
+      <c r="U7" s="30">
         <v>55.5</v>
       </c>
-      <c r="U7"/>
-      <c r="V7"/>
+      <c r="V7" s="30">
+        <v>15</v>
+      </c>
       <c r="W7"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
@@ -5303,25 +5944,32 @@
         <v>21</v>
       </c>
       <c r="N8" s="30">
+        <v>15</v>
+      </c>
+      <c r="O8" s="30">
         <v>45</v>
       </c>
-      <c r="O8" s="30">
+      <c r="P8" s="30">
         <v>60</v>
       </c>
-      <c r="P8" s="30">
+      <c r="Q8" s="30">
         <v>70.5</v>
       </c>
-      <c r="Q8" s="30">
+      <c r="R8" s="30">
+        <v>17</v>
+      </c>
+      <c r="S8" s="30">
         <v>48</v>
       </c>
-      <c r="R8" s="30">
+      <c r="T8" s="30">
         <v>59</v>
       </c>
-      <c r="S8" s="30">
+      <c r="U8" s="30">
         <v>69</v>
       </c>
-      <c r="U8"/>
-      <c r="V8"/>
+      <c r="V8" s="30">
+        <v>17</v>
+      </c>
       <c r="W8"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
@@ -5362,25 +6010,32 @@
         <v>27</v>
       </c>
       <c r="N9" s="30">
+        <v>14</v>
+      </c>
+      <c r="O9" s="30">
         <v>44</v>
       </c>
-      <c r="O9" s="30">
+      <c r="P9" s="30">
         <v>60</v>
       </c>
-      <c r="P9" s="30">
+      <c r="Q9" s="30">
         <v>78</v>
       </c>
-      <c r="Q9" s="30">
+      <c r="R9" s="30">
+        <v>15</v>
+      </c>
+      <c r="S9" s="30">
         <v>47</v>
       </c>
-      <c r="R9" s="30">
+      <c r="T9" s="30">
         <v>57</v>
       </c>
-      <c r="S9" s="30">
+      <c r="U9" s="30">
         <v>78</v>
       </c>
-      <c r="U9"/>
-      <c r="V9"/>
+      <c r="V9" s="30">
+        <v>15</v>
+      </c>
       <c r="W9"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
@@ -5421,25 +6076,32 @@
         <v>19.5</v>
       </c>
       <c r="N10" s="30">
+        <v>11</v>
+      </c>
+      <c r="O10" s="30">
         <v>45</v>
       </c>
-      <c r="O10" s="30">
+      <c r="P10" s="30">
         <v>55</v>
       </c>
-      <c r="P10" s="30">
+      <c r="Q10" s="30">
         <v>60</v>
       </c>
-      <c r="Q10" s="30">
+      <c r="R10" s="30">
+        <v>10</v>
+      </c>
+      <c r="S10" s="30">
         <v>46</v>
       </c>
-      <c r="R10" s="30">
+      <c r="T10" s="30">
         <v>56</v>
       </c>
-      <c r="S10" s="30">
+      <c r="U10" s="30">
         <v>60</v>
       </c>
-      <c r="U10"/>
-      <c r="V10"/>
+      <c r="V10" s="30">
+        <v>10</v>
+      </c>
       <c r="W10"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
@@ -5479,8 +6141,9 @@
       <c r="Q11" s="30"/>
       <c r="R11" s="30"/>
       <c r="S11" s="30"/>
-      <c r="U11"/>
-      <c r="V11"/>
+      <c r="T11" s="30"/>
+      <c r="U11" s="30"/>
+      <c r="V11" s="30"/>
       <c r="W11"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
@@ -5521,25 +6184,32 @@
         <v>10.5</v>
       </c>
       <c r="N12" s="30">
+        <v>7</v>
+      </c>
+      <c r="O12" s="30">
         <v>31</v>
       </c>
-      <c r="O12" s="30">
+      <c r="P12" s="30">
         <v>35</v>
       </c>
-      <c r="P12" s="30">
+      <c r="Q12" s="30">
         <v>40.5</v>
       </c>
-      <c r="Q12" s="30">
+      <c r="R12" s="30">
+        <v>9</v>
+      </c>
+      <c r="S12" s="30">
         <v>33</v>
       </c>
-      <c r="R12" s="30">
+      <c r="T12" s="30">
         <v>35</v>
       </c>
-      <c r="S12" s="30">
+      <c r="U12" s="30">
         <v>39</v>
       </c>
-      <c r="U12"/>
-      <c r="V12"/>
+      <c r="V12" s="30">
+        <v>9</v>
+      </c>
       <c r="W12"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
@@ -5580,25 +6250,32 @@
         <v>16.5</v>
       </c>
       <c r="N13" s="30">
+        <v>12</v>
+      </c>
+      <c r="O13" s="30">
         <v>46</v>
       </c>
-      <c r="O13" s="30">
+      <c r="P13" s="30">
         <v>55</v>
       </c>
-      <c r="P13" s="30">
+      <c r="Q13" s="30">
         <v>58.5</v>
       </c>
-      <c r="Q13" s="30">
+      <c r="R13" s="30">
+        <v>15</v>
+      </c>
+      <c r="S13" s="30">
         <v>45</v>
       </c>
-      <c r="R13" s="30">
+      <c r="T13" s="30">
         <v>55</v>
       </c>
-      <c r="S13" s="30">
+      <c r="U13" s="30">
         <v>58.5</v>
       </c>
-      <c r="U13"/>
-      <c r="V13"/>
+      <c r="V13" s="30">
+        <v>15</v>
+      </c>
       <c r="W13"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
@@ -5639,25 +6316,32 @@
         <v>22.5</v>
       </c>
       <c r="N14" s="30">
+        <v>16</v>
+      </c>
+      <c r="O14" s="30">
         <v>47</v>
       </c>
-      <c r="O14" s="30">
+      <c r="P14" s="30">
         <v>59</v>
       </c>
-      <c r="P14" s="30">
+      <c r="Q14" s="30">
         <v>72</v>
       </c>
-      <c r="Q14" s="30">
+      <c r="R14" s="30">
+        <v>18</v>
+      </c>
+      <c r="S14" s="30">
         <v>49</v>
       </c>
-      <c r="R14" s="30">
+      <c r="T14" s="30">
         <v>57</v>
       </c>
-      <c r="S14" s="30">
+      <c r="U14" s="30">
         <v>70.5</v>
       </c>
-      <c r="U14"/>
-      <c r="V14"/>
+      <c r="V14" s="30">
+        <v>18</v>
+      </c>
       <c r="W14"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
@@ -5698,25 +6382,32 @@
         <v>28.5</v>
       </c>
       <c r="N15" s="30">
+        <v>14</v>
+      </c>
+      <c r="O15" s="30">
         <v>45</v>
       </c>
-      <c r="O15" s="30">
+      <c r="P15" s="30">
         <v>60</v>
       </c>
-      <c r="P15" s="30">
+      <c r="Q15" s="30">
         <v>81</v>
       </c>
-      <c r="Q15" s="30">
+      <c r="R15" s="30">
+        <v>16</v>
+      </c>
+      <c r="S15" s="30">
         <v>49</v>
       </c>
-      <c r="R15" s="30">
+      <c r="T15" s="30">
         <v>61</v>
       </c>
-      <c r="S15" s="30">
+      <c r="U15" s="30">
         <v>78</v>
       </c>
-      <c r="U15"/>
-      <c r="V15"/>
+      <c r="V15" s="30">
+        <v>14</v>
+      </c>
       <c r="W15"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
@@ -5757,25 +6448,32 @@
         <v>19.5</v>
       </c>
       <c r="N16" s="30">
+        <v>10</v>
+      </c>
+      <c r="O16" s="30">
         <v>46</v>
       </c>
-      <c r="O16" s="30">
+      <c r="P16" s="30">
         <v>58</v>
       </c>
-      <c r="P16" s="30">
+      <c r="Q16" s="30">
         <v>61.5</v>
       </c>
-      <c r="Q16" s="30">
+      <c r="R16" s="30">
+        <v>10</v>
+      </c>
+      <c r="S16" s="30">
         <v>47</v>
       </c>
-      <c r="R16" s="30">
+      <c r="T16" s="30">
         <v>58</v>
       </c>
-      <c r="S16" s="30">
+      <c r="U16" s="30">
         <v>61.5</v>
       </c>
-      <c r="U16"/>
-      <c r="V16"/>
+      <c r="V16" s="30">
+        <v>10</v>
+      </c>
       <c r="W16"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.3">
@@ -5815,8 +6513,9 @@
       <c r="Q17" s="30"/>
       <c r="R17" s="30"/>
       <c r="S17" s="30"/>
-      <c r="U17"/>
-      <c r="V17"/>
+      <c r="T17" s="30"/>
+      <c r="U17" s="30"/>
+      <c r="V17" s="30"/>
       <c r="W17"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.3">
@@ -5857,25 +6556,32 @@
         <v>9</v>
       </c>
       <c r="N18" s="30">
+        <v>11</v>
+      </c>
+      <c r="O18" s="30">
         <v>46</v>
       </c>
-      <c r="O18" s="30">
+      <c r="P18" s="30">
         <v>49</v>
       </c>
-      <c r="P18" s="30">
+      <c r="Q18" s="30">
         <v>48</v>
       </c>
-      <c r="Q18" s="30">
+      <c r="R18" s="30">
+        <v>16</v>
+      </c>
+      <c r="S18" s="30">
         <v>51</v>
       </c>
-      <c r="R18" s="30">
+      <c r="T18" s="30">
         <v>50</v>
       </c>
-      <c r="S18" s="30">
+      <c r="U18" s="30">
         <v>52.5</v>
       </c>
-      <c r="U18"/>
-      <c r="V18"/>
+      <c r="V18" s="30">
+        <v>17</v>
+      </c>
       <c r="W18"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.3">
@@ -5916,25 +6622,32 @@
         <v>16.5</v>
       </c>
       <c r="N19" s="30">
+        <v>20</v>
+      </c>
+      <c r="O19" s="30">
         <v>66</v>
       </c>
-      <c r="O19" s="30">
+      <c r="P19" s="30">
         <v>75</v>
       </c>
-      <c r="P19" s="30">
+      <c r="Q19" s="30">
         <v>70.5</v>
       </c>
-      <c r="Q19" s="30">
+      <c r="R19" s="30">
+        <v>27</v>
+      </c>
+      <c r="S19" s="30">
         <v>71</v>
       </c>
-      <c r="R19" s="30">
+      <c r="T19" s="30">
         <v>79</v>
       </c>
-      <c r="S19" s="30">
+      <c r="U19" s="30">
         <v>76.5</v>
       </c>
-      <c r="U19"/>
-      <c r="V19"/>
+      <c r="V19" s="30">
+        <v>29</v>
+      </c>
       <c r="W19"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.3">
@@ -5975,25 +6688,32 @@
         <v>24</v>
       </c>
       <c r="N20" s="30">
+        <v>24</v>
+      </c>
+      <c r="O20" s="30">
         <v>67</v>
       </c>
-      <c r="O20" s="30">
+      <c r="P20" s="30">
         <v>85</v>
       </c>
-      <c r="P20" s="30">
+      <c r="Q20" s="30">
         <v>84</v>
       </c>
-      <c r="Q20" s="30">
+      <c r="R20" s="30">
+        <v>32</v>
+      </c>
+      <c r="S20" s="30">
         <v>75</v>
       </c>
-      <c r="R20" s="30">
+      <c r="T20" s="30">
         <v>88</v>
       </c>
-      <c r="S20" s="30">
+      <c r="U20" s="30">
         <v>90</v>
       </c>
-      <c r="U20"/>
-      <c r="V20"/>
+      <c r="V20" s="30">
+        <v>33</v>
+      </c>
       <c r="W20"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.3">
@@ -6034,25 +6754,32 @@
         <v>30</v>
       </c>
       <c r="N21" s="30">
+        <v>25</v>
+      </c>
+      <c r="O21" s="30">
         <v>68</v>
       </c>
-      <c r="O21" s="30">
+      <c r="P21" s="30">
         <v>81</v>
       </c>
-      <c r="P21" s="30">
+      <c r="Q21" s="30">
         <v>93</v>
       </c>
-      <c r="Q21" s="30">
+      <c r="R21" s="30">
+        <v>30</v>
+      </c>
+      <c r="S21" s="30">
         <v>68</v>
       </c>
-      <c r="R21" s="30">
+      <c r="T21" s="30">
         <v>86</v>
       </c>
-      <c r="S21" s="30">
+      <c r="U21" s="30">
         <v>99</v>
       </c>
-      <c r="U21"/>
-      <c r="V21"/>
+      <c r="V21" s="30">
+        <v>34</v>
+      </c>
       <c r="W21"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.3">
@@ -6093,25 +6820,32 @@
         <v>21</v>
       </c>
       <c r="N22" s="30">
+        <v>25</v>
+      </c>
+      <c r="O22" s="30">
         <v>63</v>
       </c>
-      <c r="O22" s="30">
+      <c r="P22" s="30">
         <v>77</v>
       </c>
-      <c r="P22" s="30">
+      <c r="Q22" s="30">
         <v>75</v>
       </c>
-      <c r="Q22" s="30">
+      <c r="R22" s="30">
+        <v>30</v>
+      </c>
+      <c r="S22" s="30">
         <v>70</v>
       </c>
-      <c r="R22" s="30">
+      <c r="T22" s="30">
         <v>80</v>
       </c>
-      <c r="S22" s="30">
+      <c r="U22" s="30">
         <v>81</v>
       </c>
-      <c r="U22"/>
-      <c r="V22"/>
+      <c r="V22" s="30">
+        <v>30</v>
+      </c>
       <c r="W22"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.3">
@@ -6151,8 +6885,9 @@
       <c r="Q23" s="30"/>
       <c r="R23" s="30"/>
       <c r="S23" s="30"/>
-      <c r="U23"/>
-      <c r="V23"/>
+      <c r="T23" s="30"/>
+      <c r="U23" s="30"/>
+      <c r="V23" s="30"/>
       <c r="W23"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.3">
@@ -6193,25 +6928,32 @@
         <v>12</v>
       </c>
       <c r="N24" s="30">
+        <v>15</v>
+      </c>
+      <c r="O24" s="30">
         <v>43</v>
       </c>
-      <c r="O24" s="30">
+      <c r="P24" s="30">
         <v>64</v>
       </c>
-      <c r="P24" s="30">
+      <c r="Q24" s="30">
         <v>57</v>
       </c>
-      <c r="Q24" s="30">
+      <c r="R24" s="30">
+        <v>27</v>
+      </c>
+      <c r="S24" s="30">
         <v>56</v>
       </c>
-      <c r="R24" s="30">
+      <c r="T24" s="30">
         <v>64</v>
       </c>
-      <c r="S24" s="30">
+      <c r="U24" s="30">
         <v>55.5</v>
       </c>
-      <c r="U24"/>
-      <c r="V24"/>
+      <c r="V24" s="30">
+        <v>31</v>
+      </c>
       <c r="W24"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.3">
@@ -6252,25 +6994,32 @@
         <v>21</v>
       </c>
       <c r="N25" s="30">
+        <v>25</v>
+      </c>
+      <c r="O25" s="30">
         <v>59</v>
       </c>
-      <c r="O25" s="30">
+      <c r="P25" s="30">
         <v>79</v>
       </c>
-      <c r="P25" s="30">
+      <c r="Q25" s="30">
         <v>69</v>
       </c>
-      <c r="Q25" s="30">
+      <c r="R25" s="30">
+        <v>42</v>
+      </c>
+      <c r="S25" s="30">
         <v>72</v>
       </c>
-      <c r="R25" s="30">
+      <c r="T25" s="30">
         <v>80</v>
       </c>
-      <c r="S25" s="30">
+      <c r="U25" s="30">
         <v>67.5</v>
       </c>
-      <c r="U25"/>
-      <c r="V25"/>
+      <c r="V25" s="30">
+        <v>47</v>
+      </c>
       <c r="W25"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.3">
@@ -6311,25 +7060,32 @@
         <v>27</v>
       </c>
       <c r="N26" s="30">
+        <v>31</v>
+      </c>
+      <c r="O26" s="30">
         <v>59</v>
       </c>
-      <c r="O26" s="30">
+      <c r="P26" s="30">
         <v>82</v>
       </c>
-      <c r="P26" s="30">
+      <c r="Q26" s="30">
         <v>73.5</v>
       </c>
-      <c r="Q26" s="30">
+      <c r="R26" s="30">
+        <v>51</v>
+      </c>
+      <c r="S26" s="30">
         <v>72</v>
       </c>
-      <c r="R26" s="30">
+      <c r="T26" s="30">
         <v>82</v>
       </c>
-      <c r="S26" s="30">
+      <c r="U26" s="30">
         <v>75</v>
       </c>
-      <c r="U26"/>
-      <c r="V26"/>
+      <c r="V26" s="30">
+        <v>54</v>
+      </c>
       <c r="W26"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.3">
@@ -6370,25 +7126,32 @@
         <v>33</v>
       </c>
       <c r="N27" s="30">
+        <v>32</v>
+      </c>
+      <c r="O27" s="30">
         <v>51</v>
       </c>
-      <c r="O27" s="30">
+      <c r="P27" s="30">
         <v>80</v>
       </c>
-      <c r="P27" s="30">
+      <c r="Q27" s="30">
         <v>79.5</v>
       </c>
-      <c r="Q27" s="30">
+      <c r="R27" s="30">
+        <v>49</v>
+      </c>
+      <c r="S27" s="30">
         <v>65</v>
       </c>
-      <c r="R27" s="30">
+      <c r="T27" s="30">
         <v>81</v>
       </c>
-      <c r="S27" s="30">
+      <c r="U27" s="30">
         <v>78</v>
       </c>
-      <c r="U27"/>
-      <c r="V27"/>
+      <c r="V27" s="30">
+        <v>54</v>
+      </c>
       <c r="W27"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.3">
@@ -6429,25 +7192,32 @@
         <v>22.5</v>
       </c>
       <c r="N28" s="30">
+        <v>32</v>
+      </c>
+      <c r="O28" s="30">
         <v>49</v>
       </c>
-      <c r="O28" s="30">
+      <c r="P28" s="30">
         <v>75</v>
       </c>
-      <c r="P28" s="30">
+      <c r="Q28" s="30">
         <v>66</v>
       </c>
-      <c r="Q28" s="30">
+      <c r="R28" s="30">
+        <v>49</v>
+      </c>
+      <c r="S28" s="30">
         <v>62</v>
       </c>
-      <c r="R28" s="30">
+      <c r="T28" s="30">
         <v>75</v>
       </c>
-      <c r="S28" s="30">
+      <c r="U28" s="30">
         <v>64.5</v>
       </c>
-      <c r="U28"/>
-      <c r="V28"/>
+      <c r="V28" s="30">
+        <v>53</v>
+      </c>
       <c r="W28"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.3">
@@ -6487,8 +7257,9 @@
       <c r="Q29" s="30"/>
       <c r="R29" s="30"/>
       <c r="S29" s="30"/>
-      <c r="U29"/>
-      <c r="V29"/>
+      <c r="T29" s="30"/>
+      <c r="U29" s="30"/>
+      <c r="V29" s="30"/>
       <c r="W29"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.3">
@@ -6529,25 +7300,32 @@
         <v>9</v>
       </c>
       <c r="N30" s="30">
+        <v>4</v>
+      </c>
+      <c r="O30" s="30">
         <v>26</v>
       </c>
-      <c r="O30" s="30">
+      <c r="P30" s="30">
         <v>44</v>
       </c>
-      <c r="P30" s="30">
+      <c r="Q30" s="30">
         <v>40.5</v>
       </c>
-      <c r="Q30" s="30">
+      <c r="R30" s="30">
+        <v>22</v>
+      </c>
+      <c r="S30" s="30">
         <v>30</v>
       </c>
-      <c r="R30" s="30">
+      <c r="T30" s="30">
         <v>38</v>
       </c>
-      <c r="S30" s="30">
+      <c r="U30" s="30">
         <v>40.5</v>
       </c>
-      <c r="U30"/>
-      <c r="V30"/>
+      <c r="V30" s="30">
+        <v>24</v>
+      </c>
       <c r="W30"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.3">
@@ -6588,25 +7366,32 @@
         <v>15</v>
       </c>
       <c r="N31" s="30">
+        <v>8</v>
+      </c>
+      <c r="O31" s="30">
         <v>35</v>
-      </c>
-      <c r="O31" s="30">
-        <v>45</v>
       </c>
       <c r="P31" s="30">
         <v>45</v>
       </c>
       <c r="Q31" s="30">
+        <v>45</v>
+      </c>
+      <c r="R31" s="30">
+        <v>28</v>
+      </c>
+      <c r="S31" s="30">
         <v>38</v>
       </c>
-      <c r="R31" s="30">
+      <c r="T31" s="30">
         <v>46</v>
       </c>
-      <c r="S31" s="30">
+      <c r="U31" s="30">
         <v>45</v>
       </c>
-      <c r="U31"/>
-      <c r="V31"/>
+      <c r="V31" s="30">
+        <v>32</v>
+      </c>
       <c r="W31"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.3">
@@ -6647,25 +7432,32 @@
         <v>19.5</v>
       </c>
       <c r="N32" s="30">
+        <v>11</v>
+      </c>
+      <c r="O32" s="30">
         <v>34</v>
       </c>
-      <c r="O32" s="30">
+      <c r="P32" s="30">
         <v>42</v>
       </c>
-      <c r="P32" s="30">
+      <c r="Q32" s="30">
         <v>45</v>
       </c>
-      <c r="Q32" s="30">
+      <c r="R32" s="30">
+        <v>35</v>
+      </c>
+      <c r="S32" s="30">
         <v>38</v>
       </c>
-      <c r="R32" s="30">
+      <c r="T32" s="30">
         <v>44</v>
       </c>
-      <c r="S32" s="30">
+      <c r="U32" s="30">
         <v>46.5</v>
       </c>
-      <c r="U32"/>
-      <c r="V32"/>
+      <c r="V32" s="30">
+        <v>38</v>
+      </c>
       <c r="W32"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.3">
@@ -6706,25 +7498,32 @@
         <v>22.5</v>
       </c>
       <c r="N33" s="30">
+        <v>13</v>
+      </c>
+      <c r="O33" s="30">
         <v>35</v>
       </c>
-      <c r="O33" s="30">
+      <c r="P33" s="30">
         <v>42</v>
       </c>
-      <c r="P33" s="30">
+      <c r="Q33" s="30">
         <v>46.5</v>
       </c>
-      <c r="Q33" s="30">
+      <c r="R33" s="30">
+        <v>37</v>
+      </c>
+      <c r="S33" s="30">
         <v>35</v>
       </c>
-      <c r="R33" s="30">
+      <c r="T33" s="30">
         <v>41</v>
       </c>
-      <c r="S33" s="30">
+      <c r="U33" s="30">
         <v>46.5</v>
       </c>
-      <c r="U33"/>
-      <c r="V33"/>
+      <c r="V33" s="30">
+        <v>40</v>
+      </c>
       <c r="W33"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.3">
@@ -6765,25 +7564,32 @@
         <v>16.5</v>
       </c>
       <c r="N34" s="30">
+        <v>15</v>
+      </c>
+      <c r="O34" s="30">
         <v>32</v>
       </c>
-      <c r="O34" s="30">
+      <c r="P34" s="30">
         <v>42</v>
       </c>
-      <c r="P34" s="30">
+      <c r="Q34" s="30">
         <v>37.5</v>
       </c>
-      <c r="Q34" s="30">
+      <c r="R34" s="30">
+        <v>38</v>
+      </c>
+      <c r="S34" s="30">
         <v>35</v>
       </c>
-      <c r="R34" s="30">
+      <c r="T34" s="30">
         <v>41</v>
       </c>
-      <c r="S34" s="30">
+      <c r="U34" s="30">
         <v>37.5</v>
       </c>
-      <c r="U34"/>
-      <c r="V34"/>
+      <c r="V34" s="30">
+        <v>41</v>
+      </c>
       <c r="W34"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.3">
@@ -12088,128 +12894,1976 @@
       </c>
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A227" s="25"/>
-      <c r="B227" s="21"/>
-      <c r="C227" s="21"/>
-      <c r="D227" s="21"/>
-      <c r="E227" s="21"/>
-      <c r="F227" s="21"/>
-      <c r="G227" s="21"/>
-      <c r="H227" s="28"/>
+      <c r="A227" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B227" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C227" s="21">
+        <v>1</v>
+      </c>
+      <c r="D227" s="21">
+        <v>0</v>
+      </c>
+      <c r="E227" s="21">
+        <v>1</v>
+      </c>
+      <c r="F227" s="21">
+        <v>1</v>
+      </c>
+      <c r="G227" s="21">
+        <v>0</v>
+      </c>
+      <c r="H227" s="27">
+        <v>6</v>
+      </c>
       <c r="I227" s="22"/>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A228" s="25"/>
-      <c r="B228" s="21"/>
-      <c r="C228" s="21"/>
-      <c r="D228" s="21"/>
-      <c r="E228" s="21"/>
-      <c r="F228" s="21"/>
-      <c r="G228" s="21"/>
-      <c r="H228" s="28"/>
+      <c r="A228" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B228" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C228" s="21">
+        <v>1</v>
+      </c>
+      <c r="D228" s="21">
+        <v>0</v>
+      </c>
+      <c r="E228" s="21">
+        <v>1</v>
+      </c>
+      <c r="F228" s="21">
+        <v>1</v>
+      </c>
+      <c r="G228" s="21">
+        <v>0</v>
+      </c>
+      <c r="H228" s="27">
+        <v>8</v>
+      </c>
       <c r="I228" s="22"/>
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A229" s="25"/>
-      <c r="B229" s="21"/>
-      <c r="C229" s="21"/>
-      <c r="D229" s="21"/>
-      <c r="E229" s="21"/>
-      <c r="F229" s="21"/>
-      <c r="G229" s="21"/>
-      <c r="H229" s="28"/>
+      <c r="A229" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B229" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C229" s="21">
+        <v>1</v>
+      </c>
+      <c r="D229" s="21">
+        <v>0</v>
+      </c>
+      <c r="E229" s="21">
+        <v>1</v>
+      </c>
+      <c r="F229" s="21">
+        <v>1</v>
+      </c>
+      <c r="G229" s="21">
+        <v>0</v>
+      </c>
+      <c r="H229" s="27">
+        <v>8</v>
+      </c>
       <c r="I229" s="22"/>
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A230" s="25"/>
-      <c r="B230" s="21"/>
-      <c r="C230" s="21"/>
-      <c r="D230" s="21"/>
-      <c r="E230" s="21"/>
-      <c r="F230" s="21"/>
-      <c r="G230" s="21"/>
-      <c r="H230" s="28"/>
+      <c r="A230" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B230" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C230" s="21">
+        <v>2</v>
+      </c>
+      <c r="D230" s="21">
+        <v>0</v>
+      </c>
+      <c r="E230" s="21">
+        <v>1</v>
+      </c>
+      <c r="F230" s="21">
+        <v>1</v>
+      </c>
+      <c r="G230" s="21">
+        <v>0</v>
+      </c>
+      <c r="H230" s="27">
+        <v>11</v>
+      </c>
       <c r="I230" s="22"/>
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A231" s="25"/>
-      <c r="B231" s="21"/>
-      <c r="C231" s="21"/>
-      <c r="D231" s="21"/>
-      <c r="E231" s="21"/>
-      <c r="F231" s="21"/>
-      <c r="G231" s="21"/>
-      <c r="H231" s="28"/>
+      <c r="A231" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B231" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C231" s="21">
+        <v>2</v>
+      </c>
+      <c r="D231" s="21">
+        <v>0</v>
+      </c>
+      <c r="E231" s="21">
+        <v>1</v>
+      </c>
+      <c r="F231" s="21">
+        <v>1</v>
+      </c>
+      <c r="G231" s="21">
+        <v>0</v>
+      </c>
+      <c r="H231" s="27">
+        <v>14</v>
+      </c>
       <c r="I231" s="22"/>
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A232" s="25"/>
-      <c r="B232" s="21"/>
-      <c r="C232" s="21"/>
-      <c r="D232" s="21"/>
-      <c r="E232" s="21"/>
-      <c r="F232" s="21"/>
-      <c r="G232" s="21"/>
-      <c r="H232" s="28"/>
+      <c r="A232" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B232" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C232" s="21">
+        <v>2</v>
+      </c>
+      <c r="D232" s="21">
+        <v>0</v>
+      </c>
+      <c r="E232" s="21">
+        <v>1</v>
+      </c>
+      <c r="F232" s="21">
+        <v>1</v>
+      </c>
+      <c r="G232" s="21">
+        <v>0</v>
+      </c>
+      <c r="H232" s="27">
+        <v>15</v>
+      </c>
       <c r="I232" s="22"/>
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A233" s="25"/>
-      <c r="B233" s="21"/>
-      <c r="C233" s="21"/>
-      <c r="D233" s="21"/>
-      <c r="E233" s="21"/>
-      <c r="F233" s="21"/>
-      <c r="G233" s="21"/>
-      <c r="H233" s="28"/>
+      <c r="A233" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B233" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C233" s="21">
+        <v>3</v>
+      </c>
+      <c r="D233" s="21">
+        <v>0</v>
+      </c>
+      <c r="E233" s="21">
+        <v>1</v>
+      </c>
+      <c r="F233" s="21">
+        <v>1</v>
+      </c>
+      <c r="G233" s="21">
+        <v>0</v>
+      </c>
+      <c r="H233" s="27">
+        <v>15</v>
+      </c>
       <c r="I233" s="22"/>
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A234" s="25"/>
-      <c r="B234" s="21"/>
-      <c r="C234" s="21"/>
-      <c r="D234" s="21"/>
-      <c r="E234" s="21"/>
-      <c r="F234" s="21"/>
-      <c r="G234" s="21"/>
-      <c r="H234" s="28"/>
+      <c r="A234" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B234" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C234" s="21">
+        <v>3</v>
+      </c>
+      <c r="D234" s="21">
+        <v>0</v>
+      </c>
+      <c r="E234" s="21">
+        <v>1</v>
+      </c>
+      <c r="F234" s="21">
+        <v>1</v>
+      </c>
+      <c r="G234" s="21">
+        <v>0</v>
+      </c>
+      <c r="H234" s="27">
+        <v>17</v>
+      </c>
       <c r="I234" s="22"/>
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A235" s="25"/>
-      <c r="B235" s="21"/>
-      <c r="C235" s="21"/>
-      <c r="D235" s="21"/>
-      <c r="E235" s="21"/>
-      <c r="F235" s="21"/>
+      <c r="A235" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B235" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C235" s="21">
+        <v>3</v>
+      </c>
+      <c r="D235" s="21">
+        <v>0</v>
+      </c>
+      <c r="E235" s="21">
+        <v>1</v>
+      </c>
+      <c r="F235" s="21">
+        <v>1</v>
+      </c>
+      <c r="G235" s="21">
+        <v>0</v>
+      </c>
+      <c r="H235" s="27">
+        <v>17</v>
+      </c>
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A236" s="25"/>
-      <c r="B236" s="21"/>
-      <c r="C236" s="21"/>
-      <c r="D236" s="21"/>
-      <c r="E236" s="21"/>
-      <c r="F236" s="21"/>
+      <c r="A236" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B236" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C236" s="21">
+        <v>4</v>
+      </c>
+      <c r="D236" s="21">
+        <v>0</v>
+      </c>
+      <c r="E236" s="21">
+        <v>1</v>
+      </c>
+      <c r="F236" s="21">
+        <v>1</v>
+      </c>
+      <c r="G236" s="21">
+        <v>0</v>
+      </c>
+      <c r="H236" s="27">
+        <v>14</v>
+      </c>
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A237" s="25"/>
-      <c r="B237" s="21"/>
-      <c r="C237" s="21"/>
-      <c r="D237" s="21"/>
-      <c r="E237" s="21"/>
-      <c r="F237" s="21"/>
+      <c r="A237" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B237" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C237" s="21">
+        <v>4</v>
+      </c>
+      <c r="D237" s="21">
+        <v>0</v>
+      </c>
+      <c r="E237" s="21">
+        <v>1</v>
+      </c>
+      <c r="F237" s="21">
+        <v>1</v>
+      </c>
+      <c r="G237" s="21">
+        <v>0</v>
+      </c>
+      <c r="H237" s="27">
+        <v>15</v>
+      </c>
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A238" s="25"/>
-      <c r="B238" s="21"/>
-      <c r="C238" s="21"/>
-      <c r="D238" s="21"/>
-      <c r="E238" s="21"/>
-      <c r="F238" s="21"/>
+      <c r="A238" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B238" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C238" s="21">
+        <v>4</v>
+      </c>
+      <c r="D238" s="21">
+        <v>0</v>
+      </c>
+      <c r="E238" s="21">
+        <v>1</v>
+      </c>
+      <c r="F238" s="21">
+        <v>1</v>
+      </c>
+      <c r="G238" s="21">
+        <v>0</v>
+      </c>
+      <c r="H238" s="27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A239" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B239" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C239" s="21">
+        <v>5</v>
+      </c>
+      <c r="D239" s="21">
+        <v>0</v>
+      </c>
+      <c r="E239" s="21">
+        <v>1</v>
+      </c>
+      <c r="F239" s="21">
+        <v>1</v>
+      </c>
+      <c r="G239" s="21">
+        <v>0</v>
+      </c>
+      <c r="H239" s="27">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A240" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B240" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C240" s="21">
+        <v>5</v>
+      </c>
+      <c r="D240" s="21">
+        <v>0</v>
+      </c>
+      <c r="E240" s="21">
+        <v>1</v>
+      </c>
+      <c r="F240" s="21">
+        <v>1</v>
+      </c>
+      <c r="G240" s="21">
+        <v>0</v>
+      </c>
+      <c r="H240" s="27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A241" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B241" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C241" s="21">
+        <v>5</v>
+      </c>
+      <c r="D241" s="21">
+        <v>0</v>
+      </c>
+      <c r="E241" s="21">
+        <v>1</v>
+      </c>
+      <c r="F241" s="21">
+        <v>1</v>
+      </c>
+      <c r="G241" s="21">
+        <v>0</v>
+      </c>
+      <c r="H241" s="27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A242" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B242" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C242" s="21">
+        <v>1</v>
+      </c>
+      <c r="D242" s="21">
+        <v>1</v>
+      </c>
+      <c r="E242" s="21">
+        <v>1.05</v>
+      </c>
+      <c r="F242" s="21">
+        <v>1</v>
+      </c>
+      <c r="G242" s="21">
+        <v>0.95</v>
+      </c>
+      <c r="H242" s="27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A243" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B243" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C243" s="21">
+        <v>1</v>
+      </c>
+      <c r="D243" s="21">
+        <v>1</v>
+      </c>
+      <c r="E243" s="21">
+        <v>1.05</v>
+      </c>
+      <c r="F243" s="21">
+        <v>1</v>
+      </c>
+      <c r="G243" s="21">
+        <v>0.95</v>
+      </c>
+      <c r="H243" s="27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A244" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B244" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C244" s="21">
+        <v>1</v>
+      </c>
+      <c r="D244" s="21">
+        <v>1</v>
+      </c>
+      <c r="E244" s="21">
+        <v>1.05</v>
+      </c>
+      <c r="F244" s="21">
+        <v>1</v>
+      </c>
+      <c r="G244" s="21">
+        <v>0.95</v>
+      </c>
+      <c r="H244" s="27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A245" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B245" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C245" s="21">
+        <v>2</v>
+      </c>
+      <c r="D245" s="21">
+        <v>1</v>
+      </c>
+      <c r="E245" s="21">
+        <v>1.05</v>
+      </c>
+      <c r="F245" s="21">
+        <v>1</v>
+      </c>
+      <c r="G245" s="21">
+        <v>0.95</v>
+      </c>
+      <c r="H245" s="27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A246" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B246" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C246" s="21">
+        <v>2</v>
+      </c>
+      <c r="D246" s="21">
+        <v>1</v>
+      </c>
+      <c r="E246" s="21">
+        <v>1.05</v>
+      </c>
+      <c r="F246" s="21">
+        <v>1</v>
+      </c>
+      <c r="G246" s="21">
+        <v>0.95</v>
+      </c>
+      <c r="H246" s="27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A247" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B247" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C247" s="21">
+        <v>2</v>
+      </c>
+      <c r="D247" s="21">
+        <v>1</v>
+      </c>
+      <c r="E247" s="21">
+        <v>1.05</v>
+      </c>
+      <c r="F247" s="21">
+        <v>1</v>
+      </c>
+      <c r="G247" s="21">
+        <v>0.95</v>
+      </c>
+      <c r="H247" s="27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A248" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B248" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C248" s="21">
+        <v>3</v>
+      </c>
+      <c r="D248" s="21">
+        <v>1</v>
+      </c>
+      <c r="E248" s="21">
+        <v>1.05</v>
+      </c>
+      <c r="F248" s="21">
+        <v>1</v>
+      </c>
+      <c r="G248" s="21">
+        <v>0.95</v>
+      </c>
+      <c r="H248" s="27">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A249" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B249" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C249" s="21">
+        <v>3</v>
+      </c>
+      <c r="D249" s="21">
+        <v>1</v>
+      </c>
+      <c r="E249" s="21">
+        <v>1.05</v>
+      </c>
+      <c r="F249" s="21">
+        <v>1</v>
+      </c>
+      <c r="G249" s="21">
+        <v>0.95</v>
+      </c>
+      <c r="H249" s="27">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A250" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B250" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C250" s="21">
+        <v>3</v>
+      </c>
+      <c r="D250" s="21">
+        <v>1</v>
+      </c>
+      <c r="E250" s="21">
+        <v>1.05</v>
+      </c>
+      <c r="F250" s="21">
+        <v>1</v>
+      </c>
+      <c r="G250" s="21">
+        <v>0.95</v>
+      </c>
+      <c r="H250" s="27">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A251" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B251" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C251" s="21">
+        <v>4</v>
+      </c>
+      <c r="D251" s="21">
+        <v>1</v>
+      </c>
+      <c r="E251" s="21">
+        <v>1.05</v>
+      </c>
+      <c r="F251" s="21">
+        <v>1</v>
+      </c>
+      <c r="G251" s="21">
+        <v>0.95</v>
+      </c>
+      <c r="H251" s="27">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A252" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B252" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C252" s="21">
+        <v>4</v>
+      </c>
+      <c r="D252" s="21">
+        <v>1</v>
+      </c>
+      <c r="E252" s="21">
+        <v>1.05</v>
+      </c>
+      <c r="F252" s="21">
+        <v>1</v>
+      </c>
+      <c r="G252" s="21">
+        <v>0.95</v>
+      </c>
+      <c r="H252" s="27">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A253" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B253" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C253" s="21">
+        <v>4</v>
+      </c>
+      <c r="D253" s="21">
+        <v>1</v>
+      </c>
+      <c r="E253" s="21">
+        <v>1.05</v>
+      </c>
+      <c r="F253" s="21">
+        <v>1</v>
+      </c>
+      <c r="G253" s="21">
+        <v>0.95</v>
+      </c>
+      <c r="H253" s="27">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A254" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B254" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C254" s="21">
+        <v>5</v>
+      </c>
+      <c r="D254" s="21">
+        <v>1</v>
+      </c>
+      <c r="E254" s="21">
+        <v>1.05</v>
+      </c>
+      <c r="F254" s="21">
+        <v>1</v>
+      </c>
+      <c r="G254" s="21">
+        <v>0.95</v>
+      </c>
+      <c r="H254" s="27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A255" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B255" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C255" s="21">
+        <v>5</v>
+      </c>
+      <c r="D255" s="21">
+        <v>1</v>
+      </c>
+      <c r="E255" s="21">
+        <v>1.05</v>
+      </c>
+      <c r="F255" s="21">
+        <v>1</v>
+      </c>
+      <c r="G255" s="21">
+        <v>0.95</v>
+      </c>
+      <c r="H255" s="27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A256" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B256" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C256" s="21">
+        <v>5</v>
+      </c>
+      <c r="D256" s="21">
+        <v>1</v>
+      </c>
+      <c r="E256" s="21">
+        <v>1.05</v>
+      </c>
+      <c r="F256" s="21">
+        <v>1</v>
+      </c>
+      <c r="G256" s="21">
+        <v>0.95</v>
+      </c>
+      <c r="H256" s="27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A257" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B257" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C257" s="21">
+        <v>1</v>
+      </c>
+      <c r="D257" s="21">
+        <v>2</v>
+      </c>
+      <c r="E257" s="21">
+        <v>3.04</v>
+      </c>
+      <c r="F257" s="21">
+        <v>1.96</v>
+      </c>
+      <c r="G257" s="21">
+        <v>0</v>
+      </c>
+      <c r="H257" s="27">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A258" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B258" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C258" s="21">
+        <v>1</v>
+      </c>
+      <c r="D258" s="21">
+        <v>2</v>
+      </c>
+      <c r="E258" s="21">
+        <v>3.04</v>
+      </c>
+      <c r="F258" s="21">
+        <v>1.96</v>
+      </c>
+      <c r="G258" s="21">
+        <v>0</v>
+      </c>
+      <c r="H258" s="27">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A259" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B259" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C259" s="21">
+        <v>1</v>
+      </c>
+      <c r="D259" s="21">
+        <v>2</v>
+      </c>
+      <c r="E259" s="21">
+        <v>3.04</v>
+      </c>
+      <c r="F259" s="21">
+        <v>1.96</v>
+      </c>
+      <c r="G259" s="21">
+        <v>0</v>
+      </c>
+      <c r="H259" s="27">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="260" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A260" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B260" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C260" s="21">
+        <v>2</v>
+      </c>
+      <c r="D260" s="21">
+        <v>2</v>
+      </c>
+      <c r="E260" s="21">
+        <v>3.04</v>
+      </c>
+      <c r="F260" s="21">
+        <v>1.96</v>
+      </c>
+      <c r="G260" s="21">
+        <v>0</v>
+      </c>
+      <c r="H260" s="27">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="261" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A261" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B261" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C261" s="21">
+        <v>2</v>
+      </c>
+      <c r="D261" s="21">
+        <v>2</v>
+      </c>
+      <c r="E261" s="21">
+        <v>3.04</v>
+      </c>
+      <c r="F261" s="21">
+        <v>1.96</v>
+      </c>
+      <c r="G261" s="21">
+        <v>0</v>
+      </c>
+      <c r="H261" s="27">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="262" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A262" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B262" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C262" s="21">
+        <v>2</v>
+      </c>
+      <c r="D262" s="21">
+        <v>2</v>
+      </c>
+      <c r="E262" s="21">
+        <v>3.04</v>
+      </c>
+      <c r="F262" s="21">
+        <v>1.96</v>
+      </c>
+      <c r="G262" s="21">
+        <v>0</v>
+      </c>
+      <c r="H262" s="27">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="263" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A263" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B263" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C263" s="21">
+        <v>3</v>
+      </c>
+      <c r="D263" s="21">
+        <v>2</v>
+      </c>
+      <c r="E263" s="21">
+        <v>3.04</v>
+      </c>
+      <c r="F263" s="21">
+        <v>1.96</v>
+      </c>
+      <c r="G263" s="21">
+        <v>0</v>
+      </c>
+      <c r="H263" s="27">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="264" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A264" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B264" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C264" s="21">
+        <v>3</v>
+      </c>
+      <c r="D264" s="21">
+        <v>2</v>
+      </c>
+      <c r="E264" s="21">
+        <v>3.04</v>
+      </c>
+      <c r="F264" s="21">
+        <v>1.96</v>
+      </c>
+      <c r="G264" s="21">
+        <v>0</v>
+      </c>
+      <c r="H264" s="27">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="265" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A265" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B265" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C265" s="21">
+        <v>3</v>
+      </c>
+      <c r="D265" s="21">
+        <v>2</v>
+      </c>
+      <c r="E265" s="21">
+        <v>3.04</v>
+      </c>
+      <c r="F265" s="21">
+        <v>1.96</v>
+      </c>
+      <c r="G265" s="21">
+        <v>0</v>
+      </c>
+      <c r="H265" s="27">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="266" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A266" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B266" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C266" s="21">
+        <v>4</v>
+      </c>
+      <c r="D266" s="21">
+        <v>2</v>
+      </c>
+      <c r="E266" s="21">
+        <v>3.04</v>
+      </c>
+      <c r="F266" s="21">
+        <v>1.96</v>
+      </c>
+      <c r="G266" s="21">
+        <v>0</v>
+      </c>
+      <c r="H266" s="27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="267" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A267" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B267" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C267" s="21">
+        <v>4</v>
+      </c>
+      <c r="D267" s="21">
+        <v>2</v>
+      </c>
+      <c r="E267" s="21">
+        <v>3.04</v>
+      </c>
+      <c r="F267" s="21">
+        <v>1.96</v>
+      </c>
+      <c r="G267" s="21">
+        <v>0</v>
+      </c>
+      <c r="H267" s="27">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="268" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A268" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B268" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C268" s="21">
+        <v>4</v>
+      </c>
+      <c r="D268" s="21">
+        <v>2</v>
+      </c>
+      <c r="E268" s="21">
+        <v>3.04</v>
+      </c>
+      <c r="F268" s="21">
+        <v>1.96</v>
+      </c>
+      <c r="G268" s="21">
+        <v>0</v>
+      </c>
+      <c r="H268" s="27">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="269" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A269" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B269" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C269" s="21">
+        <v>5</v>
+      </c>
+      <c r="D269" s="21">
+        <v>2</v>
+      </c>
+      <c r="E269" s="21">
+        <v>3.04</v>
+      </c>
+      <c r="F269" s="21">
+        <v>1.96</v>
+      </c>
+      <c r="G269" s="21">
+        <v>0</v>
+      </c>
+      <c r="H269" s="27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="270" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A270" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B270" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C270" s="21">
+        <v>5</v>
+      </c>
+      <c r="D270" s="21">
+        <v>2</v>
+      </c>
+      <c r="E270" s="21">
+        <v>3.04</v>
+      </c>
+      <c r="F270" s="21">
+        <v>1.96</v>
+      </c>
+      <c r="G270" s="21">
+        <v>0</v>
+      </c>
+      <c r="H270" s="27">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="271" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A271" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B271" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C271" s="21">
+        <v>5</v>
+      </c>
+      <c r="D271" s="21">
+        <v>2</v>
+      </c>
+      <c r="E271" s="21">
+        <v>3.04</v>
+      </c>
+      <c r="F271" s="21">
+        <v>1.96</v>
+      </c>
+      <c r="G271" s="21">
+        <v>0</v>
+      </c>
+      <c r="H271" s="27">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="272" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A272" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B272" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C272" s="21">
+        <v>1</v>
+      </c>
+      <c r="D272" s="21">
+        <v>3</v>
+      </c>
+      <c r="E272" s="21">
+        <v>8</v>
+      </c>
+      <c r="F272" s="21">
+        <v>3</v>
+      </c>
+      <c r="G272" s="21">
+        <v>0</v>
+      </c>
+      <c r="H272" s="28">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="273" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A273" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B273" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C273" s="21">
+        <v>1</v>
+      </c>
+      <c r="D273" s="21">
+        <v>3</v>
+      </c>
+      <c r="E273" s="21">
+        <v>8</v>
+      </c>
+      <c r="F273" s="21">
+        <v>3</v>
+      </c>
+      <c r="G273" s="21">
+        <v>0</v>
+      </c>
+      <c r="H273" s="28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="274" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A274" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B274" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C274" s="21">
+        <v>1</v>
+      </c>
+      <c r="D274" s="21">
+        <v>3</v>
+      </c>
+      <c r="E274" s="21">
+        <v>8</v>
+      </c>
+      <c r="F274" s="21">
+        <v>3</v>
+      </c>
+      <c r="G274" s="21">
+        <v>0</v>
+      </c>
+      <c r="H274" s="28">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="275" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A275" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B275" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C275" s="21">
+        <v>2</v>
+      </c>
+      <c r="D275" s="21">
+        <v>3</v>
+      </c>
+      <c r="E275" s="21">
+        <v>8</v>
+      </c>
+      <c r="F275" s="21">
+        <v>3</v>
+      </c>
+      <c r="G275" s="21">
+        <v>0</v>
+      </c>
+      <c r="H275" s="28">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="276" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A276" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B276" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C276" s="21">
+        <v>2</v>
+      </c>
+      <c r="D276" s="21">
+        <v>3</v>
+      </c>
+      <c r="E276" s="21">
+        <v>8</v>
+      </c>
+      <c r="F276" s="21">
+        <v>3</v>
+      </c>
+      <c r="G276" s="21">
+        <v>0</v>
+      </c>
+      <c r="H276" s="28">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="277" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A277" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B277" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C277" s="21">
+        <v>2</v>
+      </c>
+      <c r="D277" s="21">
+        <v>3</v>
+      </c>
+      <c r="E277" s="21">
+        <v>8</v>
+      </c>
+      <c r="F277" s="21">
+        <v>3</v>
+      </c>
+      <c r="G277" s="21">
+        <v>0</v>
+      </c>
+      <c r="H277" s="28">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="278" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A278" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B278" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C278" s="21">
+        <v>3</v>
+      </c>
+      <c r="D278" s="21">
+        <v>3</v>
+      </c>
+      <c r="E278" s="21">
+        <v>8</v>
+      </c>
+      <c r="F278" s="21">
+        <v>3</v>
+      </c>
+      <c r="G278" s="21">
+        <v>0</v>
+      </c>
+      <c r="H278" s="28">
+        <v>31</v>
+      </c>
+      <c r="I278" s="22"/>
+    </row>
+    <row r="279" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A279" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B279" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C279" s="21">
+        <v>3</v>
+      </c>
+      <c r="D279" s="21">
+        <v>3</v>
+      </c>
+      <c r="E279" s="21">
+        <v>8</v>
+      </c>
+      <c r="F279" s="21">
+        <v>3</v>
+      </c>
+      <c r="G279" s="21">
+        <v>0</v>
+      </c>
+      <c r="H279" s="28">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="280" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A280" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B280" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C280" s="21">
+        <v>3</v>
+      </c>
+      <c r="D280" s="21">
+        <v>3</v>
+      </c>
+      <c r="E280" s="21">
+        <v>8</v>
+      </c>
+      <c r="F280" s="21">
+        <v>3</v>
+      </c>
+      <c r="G280" s="21">
+        <v>0</v>
+      </c>
+      <c r="H280" s="28">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="281" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A281" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B281" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C281" s="21">
+        <v>4</v>
+      </c>
+      <c r="D281" s="21">
+        <v>3</v>
+      </c>
+      <c r="E281" s="21">
+        <v>8</v>
+      </c>
+      <c r="F281" s="21">
+        <v>3</v>
+      </c>
+      <c r="G281" s="21">
+        <v>0</v>
+      </c>
+      <c r="H281" s="28">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="282" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A282" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B282" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C282" s="21">
+        <v>4</v>
+      </c>
+      <c r="D282" s="21">
+        <v>3</v>
+      </c>
+      <c r="E282" s="21">
+        <v>8</v>
+      </c>
+      <c r="F282" s="21">
+        <v>3</v>
+      </c>
+      <c r="G282" s="21">
+        <v>0</v>
+      </c>
+      <c r="H282" s="28">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="283" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A283" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B283" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C283" s="21">
+        <v>4</v>
+      </c>
+      <c r="D283" s="21">
+        <v>3</v>
+      </c>
+      <c r="E283" s="21">
+        <v>8</v>
+      </c>
+      <c r="F283" s="21">
+        <v>3</v>
+      </c>
+      <c r="G283" s="21">
+        <v>0</v>
+      </c>
+      <c r="H283" s="28">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="284" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A284" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B284" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C284" s="21">
+        <v>5</v>
+      </c>
+      <c r="D284" s="21">
+        <v>3</v>
+      </c>
+      <c r="E284" s="21">
+        <v>8</v>
+      </c>
+      <c r="F284" s="21">
+        <v>3</v>
+      </c>
+      <c r="G284" s="21">
+        <v>0</v>
+      </c>
+      <c r="H284" s="28">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="285" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A285" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B285" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C285" s="21">
+        <v>5</v>
+      </c>
+      <c r="D285" s="21">
+        <v>3</v>
+      </c>
+      <c r="E285" s="21">
+        <v>8</v>
+      </c>
+      <c r="F285" s="21">
+        <v>3</v>
+      </c>
+      <c r="G285" s="21">
+        <v>0</v>
+      </c>
+      <c r="H285" s="28">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="286" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A286" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B286" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C286" s="21">
+        <v>5</v>
+      </c>
+      <c r="D286" s="21">
+        <v>3</v>
+      </c>
+      <c r="E286" s="21">
+        <v>8</v>
+      </c>
+      <c r="F286" s="21">
+        <v>3</v>
+      </c>
+      <c r="G286" s="21">
+        <v>0</v>
+      </c>
+      <c r="H286" s="28">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="287" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A287" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B287" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C287" s="21">
+        <v>1</v>
+      </c>
+      <c r="D287" s="21">
+        <v>4</v>
+      </c>
+      <c r="E287" s="21">
+        <v>13.7</v>
+      </c>
+      <c r="F287" s="21">
+        <v>3.97</v>
+      </c>
+      <c r="G287" s="21">
+        <v>0</v>
+      </c>
+      <c r="H287" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="288" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A288" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B288" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C288" s="21">
+        <v>1</v>
+      </c>
+      <c r="D288" s="21">
+        <v>4</v>
+      </c>
+      <c r="E288" s="21">
+        <v>13.7</v>
+      </c>
+      <c r="F288" s="21">
+        <v>3.97</v>
+      </c>
+      <c r="G288" s="21">
+        <v>0</v>
+      </c>
+      <c r="H288" s="28">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="289" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A289" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B289" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C289" s="21">
+        <v>1</v>
+      </c>
+      <c r="D289" s="21">
+        <v>4</v>
+      </c>
+      <c r="E289" s="21">
+        <v>13.7</v>
+      </c>
+      <c r="F289" s="21">
+        <v>3.97</v>
+      </c>
+      <c r="G289" s="21">
+        <v>0</v>
+      </c>
+      <c r="H289" s="28">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="290" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A290" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B290" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C290" s="21">
+        <v>2</v>
+      </c>
+      <c r="D290" s="21">
+        <v>4</v>
+      </c>
+      <c r="E290" s="21">
+        <v>13.7</v>
+      </c>
+      <c r="F290" s="21">
+        <v>3.97</v>
+      </c>
+      <c r="G290" s="21">
+        <v>0</v>
+      </c>
+      <c r="H290" s="28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="291" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A291" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B291" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C291" s="21">
+        <v>2</v>
+      </c>
+      <c r="D291" s="21">
+        <v>4</v>
+      </c>
+      <c r="E291" s="21">
+        <v>13.7</v>
+      </c>
+      <c r="F291" s="21">
+        <v>3.97</v>
+      </c>
+      <c r="G291" s="21">
+        <v>0</v>
+      </c>
+      <c r="H291" s="28">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="292" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A292" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B292" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C292" s="21">
+        <v>2</v>
+      </c>
+      <c r="D292" s="21">
+        <v>4</v>
+      </c>
+      <c r="E292" s="21">
+        <v>13.7</v>
+      </c>
+      <c r="F292" s="21">
+        <v>3.97</v>
+      </c>
+      <c r="G292" s="21">
+        <v>0</v>
+      </c>
+      <c r="H292" s="28">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="293" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A293" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B293" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C293" s="21">
+        <v>3</v>
+      </c>
+      <c r="D293" s="21">
+        <v>4</v>
+      </c>
+      <c r="E293" s="21">
+        <v>13.7</v>
+      </c>
+      <c r="F293" s="21">
+        <v>3.97</v>
+      </c>
+      <c r="G293" s="21">
+        <v>0</v>
+      </c>
+      <c r="H293" s="28">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="294" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A294" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B294" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C294" s="21">
+        <v>3</v>
+      </c>
+      <c r="D294" s="21">
+        <v>4</v>
+      </c>
+      <c r="E294" s="21">
+        <v>13.7</v>
+      </c>
+      <c r="F294" s="21">
+        <v>3.97</v>
+      </c>
+      <c r="G294" s="21">
+        <v>0</v>
+      </c>
+      <c r="H294" s="28">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="295" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A295" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B295" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C295" s="21">
+        <v>3</v>
+      </c>
+      <c r="D295" s="21">
+        <v>4</v>
+      </c>
+      <c r="E295" s="21">
+        <v>13.7</v>
+      </c>
+      <c r="F295" s="21">
+        <v>3.97</v>
+      </c>
+      <c r="G295" s="21">
+        <v>0</v>
+      </c>
+      <c r="H295" s="28">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="296" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A296" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B296" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C296" s="21">
+        <v>4</v>
+      </c>
+      <c r="D296" s="21">
+        <v>4</v>
+      </c>
+      <c r="E296" s="21">
+        <v>13.7</v>
+      </c>
+      <c r="F296" s="21">
+        <v>3.97</v>
+      </c>
+      <c r="G296" s="21">
+        <v>0</v>
+      </c>
+      <c r="H296" s="28">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="297" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A297" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B297" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C297" s="21">
+        <v>4</v>
+      </c>
+      <c r="D297" s="21">
+        <v>4</v>
+      </c>
+      <c r="E297" s="21">
+        <v>13.7</v>
+      </c>
+      <c r="F297" s="21">
+        <v>3.97</v>
+      </c>
+      <c r="G297" s="21">
+        <v>0</v>
+      </c>
+      <c r="H297" s="28">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="298" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A298" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B298" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C298" s="21">
+        <v>4</v>
+      </c>
+      <c r="D298" s="21">
+        <v>4</v>
+      </c>
+      <c r="E298" s="21">
+        <v>13.7</v>
+      </c>
+      <c r="F298" s="21">
+        <v>3.97</v>
+      </c>
+      <c r="G298" s="21">
+        <v>0</v>
+      </c>
+      <c r="H298" s="28">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="299" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A299" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B299" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C299" s="21">
+        <v>5</v>
+      </c>
+      <c r="D299" s="21">
+        <v>4</v>
+      </c>
+      <c r="E299" s="21">
+        <v>13.7</v>
+      </c>
+      <c r="F299" s="21">
+        <v>3.97</v>
+      </c>
+      <c r="G299" s="21">
+        <v>0</v>
+      </c>
+      <c r="H299" s="28">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="300" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A300" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B300" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C300" s="21">
+        <v>5</v>
+      </c>
+      <c r="D300" s="21">
+        <v>4</v>
+      </c>
+      <c r="E300" s="21">
+        <v>13.7</v>
+      </c>
+      <c r="F300" s="21">
+        <v>3.97</v>
+      </c>
+      <c r="G300" s="21">
+        <v>0</v>
+      </c>
+      <c r="H300" s="28">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="301" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A301" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B301" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C301" s="21">
+        <v>5</v>
+      </c>
+      <c r="D301" s="21">
+        <v>4</v>
+      </c>
+      <c r="E301" s="21">
+        <v>13.7</v>
+      </c>
+      <c r="F301" s="21">
+        <v>3.97</v>
+      </c>
+      <c r="G301" s="21">
+        <v>0</v>
+      </c>
+      <c r="H301" s="28">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="302" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A302" s="25"/>
+    </row>
+    <row r="303" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A303" s="25"/>
+    </row>
+    <row r="304" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A304" s="25"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting pivot="1" sqref="K5:S34">
+  <conditionalFormatting pivot="1" sqref="K5:V34">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Giving up on parallelism.  3 threads is all we get
</commit_message>
<xml_diff>
--- a/src/Simulation/Native/stats.xlsx
+++ b/src/Simulation/Native/stats.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\depot\Git\qsharp-runtime\src\Simulation\Native\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F18F7BB-C721-4F04-A7C3-AB7492191EBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA007572-0273-401E-BD80-08101EF48362}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13764" yWindow="8628" windowWidth="16080" windowHeight="10788" activeTab="1" xr2:uid="{5FEEEFE3-C5E9-4691-A26D-4009EEFDD3E5}"/>
+    <workbookView xWindow="13764" yWindow="8628" windowWidth="16080" windowHeight="10788" activeTab="3" xr2:uid="{5FEEEFE3-C5E9-4691-A26D-4009EEFDD3E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
     <sheet name="Runs" sheetId="2" r:id="rId2"/>
     <sheet name="Simple Test" sheetId="3" r:id="rId3"/>
+    <sheet name="Threading" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="12" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="61">
   <si>
     <t>Time (s)</t>
   </si>
@@ -270,6 +271,18 @@
   <si>
     <t>W15tp</t>
   </si>
+  <si>
+    <t>Fake Kernel</t>
+  </si>
+  <si>
+    <t>Real Kernel</t>
+  </si>
+  <si>
+    <t>Fake Chunked</t>
+  </si>
+  <si>
+    <t>Real Chunked</t>
+  </si>
 </sst>
 </file>
 
@@ -478,178 +491,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="76">
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
+  <dxfs count="19">
     <dxf>
       <alignment horizontal="center"/>
     </dxf>
@@ -720,6 +562,1353 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>H on 1 of 28 qubits, generic</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Threading!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fake Chunked</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Threading!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Threading!$C$2:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6538461538461537</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3076923076923075</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8076923076923075</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.3846153846153846</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.7692307692307692</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-298A-4281-B27F-6BB82231F95B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Threading!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Real Kernel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="44450">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Threading!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Threading!$E$2:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8918918918918919</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4324324324324325</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5675675675675675</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.6351351351351351</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.7702702702702702</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.8378378378378382</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-298A-4281-B27F-6BB82231F95B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Threading!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fake Kernel</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Threading!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Threading!$G$2:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2285714285714286</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2857142857142856</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2285714285714286</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1714285714285713</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0857142857142859</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-298A-4281-B27F-6BB82231F95B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Threading!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Real Chunked</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Threading!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Threading!$I$2:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9034482758620688</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3448275862068964</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3448275862068964</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.3448275862068964</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5517241379310347</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.6206896551724137</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.6206896551724137</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-298A-4281-B27F-6BB82231F95B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="990414448"/>
+        <c:axId val="1109237376"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="990414448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="8"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1109237376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1109237376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="990414448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.7481214848143992E-2"/>
+          <c:y val="0.17460718194978991"/>
+          <c:w val="0.20122789651293588"/>
+          <c:h val="0.27232854301284087"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B091860-DFAD-467F-8248-E3B9CDBA3628}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Dave Wecker" refreshedDate="43973.651789467593" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="304" xr:uid="{22FAA616-9F74-4145-9671-E5F5B83F2D90}">
   <cacheSource type="worksheet">
@@ -3832,7 +5021,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CF1768AF-73FC-4A05-B410-0579B3B8096E}" name="PivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Fusion, Thrds" colHeaderCaption=" ">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CF1768AF-73FC-4A05-B410-0579B3B8096E}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Fusion, Thrds" colHeaderCaption=" ">
   <location ref="J2:V34" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisCol" showAll="0">
@@ -4026,36 +5215,36 @@
     <dataField name="kGpS " fld="7" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
   <formats count="19">
-    <format dxfId="75">
+    <format dxfId="18">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="74">
+    <format dxfId="17">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="73">
+    <format dxfId="16">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="72">
+    <format dxfId="15">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="71">
+    <format dxfId="14">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="70">
+    <format dxfId="13">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="69">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="68">
+    <format dxfId="11">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -4065,7 +5254,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="67">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -4075,7 +5264,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="66">
+    <format dxfId="9">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -4085,29 +5274,29 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="65">
+    <format dxfId="8">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="64">
+    <format dxfId="7">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="63">
+    <format dxfId="6">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="62">
+    <format dxfId="5">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="61">
+    <format dxfId="4">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="60">
+    <format dxfId="3">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="59">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -4117,7 +5306,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="58">
+    <format dxfId="1">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -4127,7 +5316,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="57">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -5480,7 +6669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB803F0-8526-4AD8-A3BB-F38B006D6766}">
   <dimension ref="A1:W304"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
@@ -15190,4 +16379,302 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ACB03F3-1E21-47BB-8249-3AE50B9216F4}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2.6</v>
+      </c>
+      <c r="C2">
+        <f>B2/$B$2</f>
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1.48</v>
+      </c>
+      <c r="E2">
+        <f>D2/$D$2</f>
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>3.5</v>
+      </c>
+      <c r="G2">
+        <f>F2/$F$2</f>
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1.45</v>
+      </c>
+      <c r="I2">
+        <f>H2/$H$2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>4.3</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:D9" si="0">B3/$B$2</f>
+        <v>1.6538461538461537</v>
+      </c>
+      <c r="D3">
+        <v>2.8</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E9" si="1">D3/$D$2</f>
+        <v>1.8918918918918919</v>
+      </c>
+      <c r="F3">
+        <v>6.3</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G9" si="2">F3/$F$2</f>
+        <v>1.8</v>
+      </c>
+      <c r="H3">
+        <v>2.76</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I9" si="3">H3/$H$2</f>
+        <v>1.9034482758620688</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>2.3076923076923075</v>
+      </c>
+      <c r="D4">
+        <v>3.7</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="F4">
+        <v>7.8</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>2.2285714285714286</v>
+      </c>
+      <c r="H4">
+        <v>3.4</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="3"/>
+        <v>2.3448275862068964</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>7.3</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>2.8076923076923075</v>
+      </c>
+      <c r="D5">
+        <v>3.6</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>2.4324324324324325</v>
+      </c>
+      <c r="F5">
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>2.2857142857142856</v>
+      </c>
+      <c r="H5">
+        <v>3.4</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="3"/>
+        <v>2.3448275862068964</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>7.8</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>3.8</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>2.5675675675675675</v>
+      </c>
+      <c r="F6">
+        <v>7.8</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>2.2285714285714286</v>
+      </c>
+      <c r="H6">
+        <v>3.4</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="3"/>
+        <v>2.3448275862068964</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>7.8</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>3.9</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>2.6351351351351351</v>
+      </c>
+      <c r="F7">
+        <v>7.6</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>2.1714285714285713</v>
+      </c>
+      <c r="H7">
+        <v>3.7</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>2.5517241379310347</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>3.3846153846153846</v>
+      </c>
+      <c r="D8">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>2.7702702702702702</v>
+      </c>
+      <c r="F8">
+        <v>7.3</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>2.0857142857142859</v>
+      </c>
+      <c r="H8">
+        <v>3.8</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>2.6206896551724137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>3.7692307692307692</v>
+      </c>
+      <c r="D9">
+        <v>4.2</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>2.8378378378378382</v>
+      </c>
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>3.8</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>2.6206896551724137</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed generic kernel on Linux
</commit_message>
<xml_diff>
--- a/src/Simulation/Native/stats.xlsx
+++ b/src/Simulation/Native/stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\depot\Git\qsharp-runtime\src\Simulation\Native\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5DC1A9-B6D7-46E5-946B-9C8FE89B15A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1096EA-1FD7-4876-952A-8C815A59EA2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6936" yWindow="624" windowWidth="20268" windowHeight="18888" firstSheet="4" activeTab="7" xr2:uid="{5FEEEFE3-C5E9-4691-A26D-4009EEFDD3E5}"/>
+    <workbookView xWindow="6936" yWindow="624" windowWidth="20268" windowHeight="18888" firstSheet="5" activeTab="7" xr2:uid="{5FEEEFE3-C5E9-4691-A26D-4009EEFDD3E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,8 @@
     <pivotCache cacheId="0" r:id="rId9"/>
     <pivotCache cacheId="1" r:id="rId10"/>
     <pivotCache cacheId="2" r:id="rId11"/>
-    <pivotCache cacheId="10" r:id="rId12"/>
-    <pivotCache cacheId="51" r:id="rId13"/>
+    <pivotCache cacheId="3" r:id="rId12"/>
+    <pivotCache cacheId="11" r:id="rId13"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2419" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2423" uniqueCount="127">
   <si>
     <t>Time (s)</t>
   </si>
@@ -481,7 +481,13 @@
     <t>Liquid</t>
   </si>
   <si>
-    <t>Sum of Speed Up</t>
+    <t>2 d=6.1</t>
+  </si>
+  <si>
+    <t>3 d=12.1</t>
+  </si>
+  <si>
+    <t>4 d=17.0</t>
   </si>
 </sst>
 </file>
@@ -722,7 +728,55 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="286">
+  <dxfs count="172">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -749,6 +803,12 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
@@ -799,52 +859,37 @@
       <alignment horizontal="center"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
@@ -895,52 +940,37 @@
       <alignment horizontal="center"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
@@ -991,28 +1021,70 @@
       <alignment horizontal="center"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <alignment horizontal="center"/>
@@ -1061,414 +1133,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
     </dxf>
     <dxf>
       <alignment horizontal="center"/>
@@ -8276,7 +7940,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Dave Wecker" refreshedDate="43984.375722685189" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="297" xr:uid="{B4252D37-54C4-4ED0-BA45-001F17D93652}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Dave Wecker" refreshedDate="43984.678717476854" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="297" xr:uid="{B4252D37-54C4-4ED0-BA45-001F17D93652}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:I1048576" sheet="Fusion (4)"/>
   </cacheSource>
@@ -17852,8 +17516,8 @@
     <x v="0"/>
     <n v="1.03"/>
     <n v="11"/>
-    <n v="33.9"/>
-    <n v="0.32448377581120946"/>
+    <n v="36"/>
+    <n v="0.30555555555555558"/>
   </r>
   <r>
     <x v="1"/>
@@ -19434,20 +19098,20 @@
     <x v="1"/>
     <x v="0"/>
     <x v="0"/>
-    <n v="1.95"/>
-    <n v="5.2"/>
-    <n v="14"/>
-    <n v="0.37142857142857144"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <n v="1.95"/>
-    <n v="14"/>
-    <n v="14"/>
+    <n v="1.19"/>
+    <n v="14.1"/>
+    <n v="21"/>
+    <n v="0.67142857142857137"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1.18"/>
+    <n v="21"/>
+    <n v="21"/>
     <n v="1"/>
   </r>
   <r>
@@ -19456,505 +19120,505 @@
     <x v="1"/>
     <x v="0"/>
     <x v="0"/>
-    <n v="1.95"/>
-    <n v="16.399999999999999"/>
-    <n v="14"/>
-    <n v="1.1714285714285713"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="1.95"/>
-    <n v="9.1999999999999993"/>
-    <n v="14"/>
-    <n v="0.65714285714285714"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="1.95"/>
+    <n v="1.18"/>
+    <n v="19.600000000000001"/>
+    <n v="21"/>
+    <n v="0.93333333333333335"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="1.19"/>
+    <n v="27.1"/>
+    <n v="21"/>
+    <n v="1.2904761904761906"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="1.18"/>
+    <n v="34.4"/>
+    <n v="21"/>
+    <n v="1.638095238095238"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="1.19"/>
+    <n v="33.5"/>
+    <n v="21"/>
+    <n v="1.5952380952380953"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="1.18"/>
+    <n v="23.5"/>
+    <n v="21"/>
+    <n v="1.1190476190476191"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="1.18"/>
+    <n v="34.9"/>
+    <n v="21"/>
+    <n v="1.6619047619047618"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="1.18"/>
+    <n v="34.5"/>
+    <n v="21"/>
+    <n v="1.6428571428571428"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="1.18"/>
+    <n v="31.4"/>
+    <n v="21"/>
+    <n v="1.4952380952380953"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="1.19"/>
+    <n v="37.9"/>
+    <n v="21"/>
+    <n v="1.8047619047619048"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="1.19"/>
+    <n v="36.9"/>
+    <n v="21"/>
+    <n v="1.7571428571428571"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="6.2"/>
+    <n v="45.3"/>
+    <n v="21"/>
+    <n v="2.157142857142857"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="6.2"/>
+    <n v="76.8"/>
+    <n v="21"/>
+    <n v="3.657142857142857"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="6.2"/>
+    <n v="75.7"/>
+    <n v="21"/>
+    <n v="3.6047619047619048"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="6.21"/>
+    <n v="83.7"/>
+    <n v="21"/>
+    <n v="3.9857142857142858"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="6.2"/>
+    <n v="130.30000000000001"/>
+    <n v="21"/>
+    <n v="6.2047619047619049"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="6.2"/>
+    <n v="140.4"/>
+    <n v="21"/>
+    <n v="6.6857142857142859"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="6.21"/>
+    <n v="112.7"/>
+    <n v="21"/>
+    <n v="5.3666666666666671"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="6.2"/>
+    <n v="163.80000000000001"/>
+    <n v="21"/>
+    <n v="7.8000000000000007"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="6.2"/>
+    <n v="146.19999999999999"/>
+    <n v="21"/>
+    <n v="6.9619047619047612"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="6.2"/>
+    <n v="104.7"/>
+    <n v="21"/>
+    <n v="4.9857142857142858"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="6.2"/>
+    <n v="165.3"/>
+    <n v="21"/>
+    <n v="7.8714285714285719"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="6.2"/>
+    <n v="149.69999999999999"/>
+    <n v="21"/>
+    <n v="7.1285714285714281"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="12.04"/>
+    <n v="14.6"/>
+    <n v="21"/>
+    <n v="0.69523809523809521"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="11.93"/>
+    <n v="67"/>
+    <n v="21"/>
+    <n v="3.1904761904761907"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="11.94"/>
+    <n v="73.5"/>
+    <n v="21"/>
+    <n v="3.5"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="11.95"/>
+    <n v="32.5"/>
+    <n v="21"/>
+    <n v="1.5476190476190477"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="11.93"/>
+    <n v="131.69999999999999"/>
+    <n v="21"/>
+    <n v="6.2714285714285705"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="11.93"/>
+    <n v="132.19999999999999"/>
+    <n v="21"/>
+    <n v="6.2952380952380951"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="11.96"/>
+    <n v="42.3"/>
+    <n v="21"/>
+    <n v="2.0142857142857142"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="11.93"/>
+    <n v="154.80000000000001"/>
+    <n v="21"/>
+    <n v="7.3714285714285719"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="11.93"/>
+    <n v="160.80000000000001"/>
+    <n v="21"/>
+    <n v="7.6571428571428575"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="11.96"/>
+    <n v="47.6"/>
+    <n v="21"/>
+    <n v="2.2666666666666666"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="11.93"/>
+    <n v="168.1"/>
+    <n v="21"/>
+    <n v="8.0047619047619047"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="11.93"/>
+    <n v="155.6"/>
+    <n v="21"/>
+    <n v="7.409523809523809"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="18.260000000000002"/>
+    <n v="10.6"/>
+    <n v="21"/>
+    <n v="0.50476190476190474"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="18.239999999999998"/>
+    <n v="70.099999999999994"/>
+    <n v="21"/>
+    <n v="3.3380952380952378"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="18.23"/>
+    <n v="69"/>
+    <n v="21"/>
+    <n v="3.2857142857142856"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="18.260000000000002"/>
     <n v="21.1"/>
-    <n v="14"/>
-    <n v="1.5071428571428573"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="1.95"/>
-    <n v="28.5"/>
-    <n v="14"/>
-    <n v="2.0357142857142856"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="0"/>
-    <n v="1.95"/>
-    <n v="10.3"/>
-    <n v="14"/>
-    <n v="0.73571428571428577"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="0"/>
-    <n v="1.95"/>
-    <n v="32.5"/>
-    <n v="14"/>
-    <n v="2.3214285714285716"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="0"/>
-    <n v="1.95"/>
-    <n v="34.200000000000003"/>
-    <n v="14"/>
-    <n v="2.4428571428571431"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="3"/>
-    <x v="0"/>
-    <n v="1.95"/>
-    <n v="13.3"/>
-    <n v="14"/>
-    <n v="0.95000000000000007"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="3"/>
-    <x v="0"/>
-    <n v="1.95"/>
-    <n v="37.200000000000003"/>
-    <n v="14"/>
-    <n v="2.6571428571428575"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="3"/>
-    <x v="0"/>
-    <n v="1.95"/>
-    <n v="37.200000000000003"/>
-    <n v="14"/>
-    <n v="2.6571428571428575"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <n v="1.88"/>
-    <n v="19.8"/>
-    <n v="14"/>
-    <n v="1.4142857142857144"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <n v="1.89"/>
-    <n v="65.900000000000006"/>
-    <n v="14"/>
-    <n v="4.7071428571428573"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <n v="1.89"/>
-    <n v="66.2"/>
-    <n v="14"/>
-    <n v="4.7285714285714286"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <n v="1.89"/>
-    <n v="35.6"/>
-    <n v="14"/>
-    <n v="2.5428571428571431"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <n v="1.89"/>
-    <n v="112.5"/>
-    <n v="14"/>
-    <n v="8.0357142857142865"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <n v="1.89"/>
-    <n v="127.6"/>
-    <n v="14"/>
-    <n v="9.1142857142857139"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="1"/>
-    <n v="1.89"/>
-    <n v="48.6"/>
-    <n v="14"/>
-    <n v="3.4714285714285715"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="1"/>
-    <n v="1.89"/>
-    <n v="134.5"/>
-    <n v="14"/>
-    <n v="9.6071428571428577"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="1"/>
-    <n v="1.89"/>
-    <n v="114.5"/>
-    <n v="14"/>
-    <n v="8.1785714285714288"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="3"/>
-    <x v="1"/>
-    <n v="1.89"/>
-    <n v="35.5"/>
-    <n v="14"/>
-    <n v="2.5357142857142856"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="3"/>
-    <x v="1"/>
-    <n v="1.89"/>
-    <n v="120.2"/>
-    <n v="14"/>
-    <n v="8.5857142857142854"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="3"/>
-    <x v="1"/>
-    <n v="1.89"/>
-    <n v="150.1"/>
-    <n v="14"/>
-    <n v="10.721428571428572"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <n v="3"/>
-    <n v="6.2"/>
-    <n v="14"/>
-    <n v="0.44285714285714289"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <n v="3"/>
-    <n v="46.9"/>
-    <n v="14"/>
-    <n v="3.35"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <n v="3"/>
-    <n v="50.8"/>
-    <n v="14"/>
-    <n v="3.6285714285714286"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
-    <n v="3"/>
-    <n v="11"/>
-    <n v="14"/>
-    <n v="0.7857142857142857"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
-    <n v="3"/>
-    <n v="101.2"/>
-    <n v="14"/>
-    <n v="7.2285714285714286"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
-    <n v="3"/>
-    <n v="79.5"/>
-    <n v="14"/>
-    <n v="5.6785714285714288"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
-    <n v="3"/>
-    <n v="18.399999999999999"/>
-    <n v="14"/>
-    <n v="1.3142857142857143"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
-    <n v="3"/>
-    <n v="109"/>
-    <n v="14"/>
-    <n v="7.7857142857142856"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
-    <n v="3"/>
-    <n v="100.5"/>
-    <n v="14"/>
-    <n v="7.1785714285714288"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="3"/>
-    <x v="2"/>
-    <n v="3"/>
-    <n v="20.3"/>
-    <n v="14"/>
-    <n v="1.45"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="3"/>
-    <x v="2"/>
-    <n v="3"/>
-    <n v="112.4"/>
-    <n v="14"/>
-    <n v="8.0285714285714285"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="3"/>
-    <x v="2"/>
-    <n v="3"/>
-    <n v="111.6"/>
-    <n v="14"/>
-    <n v="7.9714285714285706"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="3"/>
-    <n v="3.86"/>
-    <n v="5.2"/>
-    <n v="14"/>
-    <n v="0.37142857142857144"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="3"/>
-    <n v="3.86"/>
-    <n v="54.3"/>
-    <n v="14"/>
-    <n v="3.8785714285714286"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="3"/>
-    <n v="3.85"/>
-    <n v="55.1"/>
-    <n v="14"/>
-    <n v="3.9357142857142859"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="3"/>
-    <n v="3.85"/>
-    <n v="5.9"/>
-    <n v="14"/>
-    <n v="0.42142857142857143"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="3"/>
-    <n v="3.86"/>
-    <n v="103.5"/>
-    <n v="14"/>
-    <n v="7.3928571428571432"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="3"/>
-    <n v="3.86"/>
-    <n v="104.5"/>
-    <n v="14"/>
-    <n v="7.4642857142857144"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="3"/>
-    <n v="3.84"/>
-    <n v="11"/>
-    <n v="14"/>
-    <n v="0.7857142857142857"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="3"/>
-    <n v="3.86"/>
-    <n v="111"/>
-    <n v="14"/>
-    <n v="7.9285714285714288"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="3"/>
-    <n v="3.86"/>
-    <n v="111.4"/>
-    <n v="14"/>
-    <n v="7.9571428571428573"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="3"/>
-    <x v="3"/>
-    <n v="3.86"/>
-    <n v="12.3"/>
-    <n v="14"/>
-    <n v="0.87857142857142867"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="3"/>
-    <x v="3"/>
-    <n v="3.86"/>
-    <n v="124.7"/>
-    <n v="14"/>
-    <n v="8.9071428571428566"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="3"/>
-    <x v="3"/>
-    <n v="3.86"/>
-    <n v="123.9"/>
-    <n v="14"/>
-    <n v="8.85"/>
+    <n v="21"/>
+    <n v="1.0047619047619047"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="18.239999999999998"/>
+    <n v="129.4"/>
+    <n v="21"/>
+    <n v="6.1619047619047622"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="18.23"/>
+    <n v="122.6"/>
+    <n v="21"/>
+    <n v="5.8380952380952378"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="18.25"/>
+    <n v="26.2"/>
+    <n v="21"/>
+    <n v="1.2476190476190476"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="18.239999999999998"/>
+    <n v="150.6"/>
+    <n v="21"/>
+    <n v="7.1714285714285708"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="18.22"/>
+    <n v="149.9"/>
+    <n v="21"/>
+    <n v="7.1380952380952385"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="18.23"/>
+    <n v="29.2"/>
+    <n v="21"/>
+    <n v="1.3904761904761904"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="18.23"/>
+    <n v="167.2"/>
+    <n v="21"/>
+    <n v="7.9619047619047612"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="18.23"/>
+    <n v="165"/>
+    <n v="21"/>
+    <n v="7.8571428571428568"/>
   </r>
   <r>
     <x v="2"/>
@@ -20749,36 +20413,36 @@
     <dataField name="kGpS " fld="7" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
   <formats count="19">
-    <format dxfId="285">
+    <format dxfId="171">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="284">
+    <format dxfId="170">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="283">
+    <format dxfId="169">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="282">
+    <format dxfId="168">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="281">
+    <format dxfId="167">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="280">
+    <format dxfId="166">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="279">
+    <format dxfId="165">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="278">
+    <format dxfId="164">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -20788,7 +20452,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="277">
+    <format dxfId="163">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -20798,7 +20462,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="276">
+    <format dxfId="162">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -20808,29 +20472,29 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="275">
+    <format dxfId="161">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="274">
+    <format dxfId="160">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="273">
+    <format dxfId="159">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="272">
+    <format dxfId="158">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="271">
+    <format dxfId="157">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="270">
+    <format dxfId="156">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="269">
+    <format dxfId="155">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -20840,7 +20504,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="268">
+    <format dxfId="154">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -20850,7 +20514,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="267">
+    <format dxfId="153">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -21164,7 +20828,7 @@
     <dataField name="Speed Up " fld="6" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="266">
+    <format dxfId="152">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -21447,7 +21111,7 @@
     <dataField name="Speed Up " fld="6" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="265">
+    <format dxfId="151">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -21566,7 +21230,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C1D42410-11DD-49F8-AAE0-94EA0CBF909A}" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Width, Thrds" colHeaderCaption="Qs">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C1D42410-11DD-49F8-AAE0-94EA0CBF909A}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Width, Thrds" colHeaderCaption="Qs">
   <location ref="L2:X25" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
@@ -21737,26 +21401,26 @@
     <dataField name="Speed Up " fld="8" subtotal="average" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="16">
-    <format dxfId="264">
+    <format dxfId="150">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="263">
+    <format dxfId="149">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="262">
+    <format dxfId="148">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="2"/>
     </format>
-    <format dxfId="261">
+    <format dxfId="147">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="260">
+    <format dxfId="146">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="259">
+    <format dxfId="145">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -21770,7 +21434,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="258">
+    <format dxfId="144">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -21784,7 +21448,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="257">
+    <format dxfId="143">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -21798,26 +21462,26 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="256">
+    <format dxfId="142">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="255">
+    <format dxfId="141">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="254">
+    <format dxfId="140">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="2"/>
     </format>
-    <format dxfId="253">
+    <format dxfId="139">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="252">
+    <format dxfId="138">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="251">
+    <format dxfId="137">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -21831,7 +21495,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="250">
+    <format dxfId="136">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -21845,7 +21509,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="249">
+    <format dxfId="135">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -21886,25 +21550,24 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{872FE7F9-99AF-4A71-AE57-226758E0BB48}" name="PivotTable1" cacheId="51" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Width, Thrds" colHeaderCaption="Qs">
-  <location ref="L2:P25" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{872FE7F9-99AF-4A71-AE57-226758E0BB48}" name="PivotTable1" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Width, Thrds" colHeaderCaption="Qs">
+  <location ref="L2:R25" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
       <items count="4">
+        <item x="1"/>
         <item x="0"/>
-        <item h="1" x="1"/>
         <item h="1" x="2"/>
         <item h="1" x="3"/>
       </items>
     </pivotField>
-    <pivotField axis="axisCol" showAll="0" nonAutoSortDefault="1">
-      <items count="6">
+    <pivotField axis="axisCol" showAll="0" nonAutoSortDefault="1" defaultSubtotal="0">
+      <items count="5">
         <item n="Gen" h="1" x="0"/>
         <item h="1" x="1"/>
         <item x="2"/>
         <item h="1" x="4"/>
         <item x="3"/>
-        <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
@@ -21927,9 +21590,9 @@
     <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
       <items count="5">
         <item n="1 d=1.2" x="0"/>
-        <item n="2 d=5.6" x="1"/>
-        <item n="3 d=10.0" x="2"/>
-        <item n="4 d=14.4" x="3"/>
+        <item n="2 d=6.1" x="1"/>
+        <item n="3 d=12.1" x="2"/>
+        <item n="4 d=17.0" x="3"/>
         <item h="1" x="4"/>
       </items>
     </pivotField>
@@ -22009,10 +21672,14 @@
     <field x="0"/>
     <field x="1"/>
   </colFields>
-  <colItems count="4">
+  <colItems count="6">
     <i>
       <x/>
       <x/>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
       <x v="2"/>
     </i>
     <i r="2">
@@ -22023,34 +21690,52 @@
       <x/>
       <x v="2"/>
     </i>
+    <i r="1">
+      <x v="1"/>
+      <x v="2"/>
+    </i>
     <i r="2">
       <x v="4"/>
     </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Sum of Speed Up" fld="8" baseField="0" baseItem="0" numFmtId="2"/>
+    <dataField name="Speed Up " fld="8" baseField="0" baseItem="0" numFmtId="2"/>
   </dataFields>
-  <formats count="25">
-    <format dxfId="201">
+  <formats count="27">
+    <format dxfId="134">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="202">
+    <format dxfId="133">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="203">
+    <format dxfId="132">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="2"/>
     </format>
-    <format dxfId="204">
+    <format dxfId="131">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="205">
+    <format dxfId="130">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="206">
+    <format dxfId="129">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="3">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="128">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -22064,7 +21749,40 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="207">
+    <format dxfId="127">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="1" count="3">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="126">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="125">
+      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
+    </format>
+    <format dxfId="124">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="2"/>
+    </format>
+    <format dxfId="123">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="122">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="121">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -22078,7 +21796,21 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="208">
+    <format dxfId="120">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="3">
+            <x v="0"/>
+            <x v="1"/>
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="119">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -22092,83 +21824,22 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="209">
+    <format dxfId="118">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="210">
+    <format dxfId="117">
+      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="116">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="211">
+    <format dxfId="115">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="2"/>
     </format>
-    <format dxfId="212">
+    <format dxfId="114">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="213">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="214">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="3">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="215">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="3">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="216">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="2">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="1" count="3">
-            <x v="0"/>
-            <x v="1"/>
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="8">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="7">
-      <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
-    </format>
-    <format dxfId="6">
-      <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
-    </format>
-    <format dxfId="5">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="2"/>
-    </format>
-    <format dxfId="4">
-      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="3">
+    <format dxfId="113">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="2">
@@ -22178,7 +21849,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="112">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="0"/>
@@ -22188,7 +21859,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="111">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="0" selected="0"/>
@@ -22199,12 +21870,30 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="110">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="0" selected="0"/>
           <reference field="1" count="0"/>
           <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="109">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="2" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="108">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="2" count="1">
             <x v="1"/>
           </reference>
         </references>
@@ -53316,9 +53005,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D8DB23A-8D81-4433-B1C6-7993A3C53A82}">
   <dimension ref="A1:AL297"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M42" sqref="M42"/>
+      <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -53328,12 +53017,12 @@
     <col min="6" max="6" width="11" style="11" customWidth="1"/>
     <col min="7" max="10" width="8.88671875" style="11"/>
     <col min="11" max="11" width="15.77734375" style="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.77734375" style="40" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.109375" style="40" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.77734375" style="40" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.109375" style="40" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.5546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" style="40" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.77734375" style="40" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.109375" style="40" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.6640625" style="40" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.77734375" style="40" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="6.109375" style="40" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="5.5546875" style="40" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="6.77734375" style="40" bestFit="1" customWidth="1"/>
@@ -53436,7 +53125,7 @@
       </c>
       <c r="K2" s="31"/>
       <c r="L2" s="36" t="s">
-        <v>124</v>
+        <v>69</v>
       </c>
       <c r="M2" s="47" t="s">
         <v>100</v>
@@ -53444,8 +53133,8 @@
       <c r="N2" s="42"/>
       <c r="O2" s="42"/>
       <c r="P2" s="42"/>
-      <c r="Q2"/>
-      <c r="R2"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="42"/>
       <c r="S2"/>
       <c r="T2"/>
       <c r="U2"/>
@@ -53492,16 +53181,16 @@
       </c>
       <c r="K3"/>
       <c r="L3"/>
-      <c r="M3" s="11">
+      <c r="M3" s="29">
         <v>15</v>
       </c>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11">
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29">
         <v>26</v>
       </c>
-      <c r="P3" s="11"/>
-      <c r="Q3"/>
-      <c r="R3"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
       <c r="S3"/>
       <c r="T3"/>
       <c r="U3"/>
@@ -53552,15 +53241,18 @@
       <c r="K4"/>
       <c r="L4"/>
       <c r="M4" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="N4" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="N4" s="42"/>
-      <c r="O4" s="42" t="s">
+      <c r="O4" s="42"/>
+      <c r="P4" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q4" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="P4" s="42"/>
-      <c r="Q4"/>
-      <c r="R4"/>
       <c r="S4"/>
       <c r="T4"/>
       <c r="U4"/>
@@ -53615,17 +53307,21 @@
       <c r="M5" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="N5" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="O5" s="42" t="s">
+      <c r="P5" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="P5" s="11" t="s">
+      <c r="Q5" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="R5" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="Q5"/>
-      <c r="R5"/>
       <c r="S5"/>
       <c r="T5"/>
       <c r="U5"/>
@@ -53681,8 +53377,8 @@
       <c r="N6" s="42"/>
       <c r="O6" s="42"/>
       <c r="P6" s="42"/>
-      <c r="Q6"/>
-      <c r="R6"/>
+      <c r="Q6" s="42"/>
+      <c r="R6" s="42"/>
       <c r="S6"/>
       <c r="T6"/>
       <c r="U6"/>
@@ -53735,15 +53431,19 @@
         <v>1</v>
       </c>
       <c r="M7" s="42">
+        <v>0.97222222222222221</v>
+      </c>
+      <c r="N7" s="42">
         <v>1.0914454277286136</v>
       </c>
-      <c r="N7" s="42"/>
-      <c r="O7" s="42">
+      <c r="O7" s="42"/>
+      <c r="P7" s="42">
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="Q7" s="42">
         <v>1.0440251572327044</v>
       </c>
-      <c r="P7" s="42"/>
-      <c r="Q7"/>
-      <c r="R7"/>
+      <c r="R7" s="42"/>
       <c r="S7"/>
       <c r="T7"/>
       <c r="U7"/>
@@ -53796,15 +53496,19 @@
         <v>2</v>
       </c>
       <c r="M8" s="42">
+        <v>1.5277777777777777</v>
+      </c>
+      <c r="N8" s="42">
         <v>1.5486725663716814</v>
       </c>
-      <c r="N8" s="42"/>
-      <c r="O8" s="42">
+      <c r="O8" s="42"/>
+      <c r="P8" s="42">
+        <v>1.5952380952380953</v>
+      </c>
+      <c r="Q8" s="42">
         <v>1.6037735849056602</v>
       </c>
-      <c r="P8" s="42"/>
-      <c r="Q8"/>
-      <c r="R8"/>
+      <c r="R8" s="42"/>
       <c r="S8"/>
       <c r="T8"/>
       <c r="U8"/>
@@ -53857,15 +53561,19 @@
         <v>3</v>
       </c>
       <c r="M9" s="42">
+        <v>1.8055555555555556</v>
+      </c>
+      <c r="N9" s="42">
         <v>1.6991150442477878</v>
       </c>
-      <c r="N9" s="42"/>
-      <c r="O9" s="42">
+      <c r="O9" s="42"/>
+      <c r="P9" s="42">
+        <v>1.6428571428571428</v>
+      </c>
+      <c r="Q9" s="42">
         <v>2.1446540880503147</v>
       </c>
-      <c r="P9" s="42"/>
-      <c r="Q9"/>
-      <c r="R9"/>
+      <c r="R9" s="42"/>
       <c r="S9"/>
       <c r="T9"/>
       <c r="U9"/>
@@ -53918,19 +53626,23 @@
         <v>4</v>
       </c>
       <c r="M10" s="42">
+        <v>1.9166666666666667</v>
+      </c>
+      <c r="N10" s="42">
         <v>1.7256637168141593</v>
       </c>
-      <c r="N10" s="42">
+      <c r="O10" s="42">
         <v>4.4247787610619468E-2</v>
       </c>
-      <c r="O10" s="42">
+      <c r="P10" s="42">
+        <v>1.7571428571428571</v>
+      </c>
+      <c r="Q10" s="42">
         <v>2.2578616352201255</v>
       </c>
-      <c r="P10" s="42">
+      <c r="R10" s="42">
         <v>3.7735849056603772E-2</v>
       </c>
-      <c r="Q10"/>
-      <c r="R10"/>
       <c r="S10"/>
       <c r="T10"/>
       <c r="U10"/>
@@ -53980,14 +53692,14 @@
       </c>
       <c r="K11"/>
       <c r="L11" s="23" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="M11" s="42"/>
       <c r="N11" s="42"/>
       <c r="O11" s="42"/>
       <c r="P11" s="42"/>
-      <c r="Q11"/>
-      <c r="R11"/>
+      <c r="Q11" s="42"/>
+      <c r="R11" s="42"/>
       <c r="S11"/>
       <c r="T11"/>
       <c r="U11"/>
@@ -54040,15 +53752,19 @@
         <v>1</v>
       </c>
       <c r="M12" s="42">
+        <v>3.7222222222222223</v>
+      </c>
+      <c r="N12" s="42">
         <v>3.9498525073746316</v>
       </c>
-      <c r="N12" s="42"/>
-      <c r="O12" s="42">
+      <c r="O12" s="42"/>
+      <c r="P12" s="42">
+        <v>3.6047619047619048</v>
+      </c>
+      <c r="Q12" s="42">
         <v>4.7295597484276728</v>
       </c>
-      <c r="P12" s="42"/>
-      <c r="Q12"/>
-      <c r="R12"/>
+      <c r="R12" s="42"/>
       <c r="S12"/>
       <c r="T12"/>
       <c r="U12"/>
@@ -54101,15 +53817,19 @@
         <v>2</v>
       </c>
       <c r="M13" s="42">
+        <v>4.8888888888888893</v>
+      </c>
+      <c r="N13" s="42">
         <v>4.3893805309734519</v>
       </c>
-      <c r="N13" s="42"/>
-      <c r="O13" s="42">
+      <c r="O13" s="42"/>
+      <c r="P13" s="42">
+        <v>6.6857142857142859</v>
+      </c>
+      <c r="Q13" s="42">
         <v>8.0440251572327046</v>
       </c>
-      <c r="P13" s="42"/>
-      <c r="Q13"/>
-      <c r="R13"/>
+      <c r="R13" s="42"/>
       <c r="S13"/>
       <c r="T13"/>
       <c r="U13"/>
@@ -54162,15 +53882,19 @@
         <v>3</v>
       </c>
       <c r="M14" s="42">
+        <v>5.5555555555555554</v>
+      </c>
+      <c r="N14" s="42">
         <v>4.1032448377581119</v>
       </c>
-      <c r="N14" s="42"/>
-      <c r="O14" s="42">
+      <c r="O14" s="42"/>
+      <c r="P14" s="42">
+        <v>6.9619047619047612</v>
+      </c>
+      <c r="Q14" s="42">
         <v>9.3459119496855347</v>
       </c>
-      <c r="P14" s="42"/>
-      <c r="Q14"/>
-      <c r="R14"/>
+      <c r="R14" s="42"/>
       <c r="S14"/>
       <c r="T14"/>
       <c r="U14"/>
@@ -54223,19 +53947,23 @@
         <v>4</v>
       </c>
       <c r="M15" s="42">
+        <v>5.583333333333333</v>
+      </c>
+      <c r="N15" s="42">
         <v>4.3274336283185839</v>
       </c>
-      <c r="N15" s="42">
+      <c r="O15" s="42">
         <v>7.6696165191740412E-2</v>
       </c>
-      <c r="O15" s="42">
+      <c r="P15" s="42">
+        <v>7.1285714285714281</v>
+      </c>
+      <c r="Q15" s="42">
         <v>9.5031446540880502</v>
       </c>
-      <c r="P15" s="42">
+      <c r="R15" s="42">
         <v>5.0314465408805034E-2</v>
       </c>
-      <c r="Q15"/>
-      <c r="R15"/>
       <c r="S15"/>
       <c r="T15"/>
       <c r="U15"/>
@@ -54285,14 +54013,14 @@
       </c>
       <c r="K16"/>
       <c r="L16" s="23" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="M16" s="42"/>
       <c r="N16" s="42"/>
       <c r="O16" s="42"/>
       <c r="P16" s="42"/>
-      <c r="Q16"/>
-      <c r="R16"/>
+      <c r="Q16" s="42"/>
+      <c r="R16" s="42"/>
       <c r="S16"/>
       <c r="T16"/>
       <c r="U16"/>
@@ -54345,15 +54073,19 @@
         <v>1</v>
       </c>
       <c r="M17" s="42">
+        <v>2.4166666666666665</v>
+      </c>
+      <c r="N17" s="42">
         <v>2.3392330383480826</v>
       </c>
-      <c r="N17" s="42"/>
-      <c r="O17" s="42">
+      <c r="O17" s="42"/>
+      <c r="P17" s="42">
+        <v>3.5</v>
+      </c>
+      <c r="Q17" s="42">
         <v>3.742138364779874</v>
       </c>
-      <c r="P17" s="42"/>
-      <c r="Q17"/>
-      <c r="R17"/>
+      <c r="R17" s="42"/>
       <c r="S17"/>
       <c r="T17"/>
       <c r="U17"/>
@@ -54406,15 +54138,19 @@
         <v>2</v>
       </c>
       <c r="M18" s="42">
+        <v>3.6388888888888888</v>
+      </c>
+      <c r="N18" s="42">
         <v>2.7699115044247788</v>
       </c>
-      <c r="N18" s="42"/>
-      <c r="O18" s="42">
+      <c r="O18" s="42"/>
+      <c r="P18" s="42">
+        <v>6.2952380952380951</v>
+      </c>
+      <c r="Q18" s="42">
         <v>6.6352201257861632</v>
       </c>
-      <c r="P18" s="42"/>
-      <c r="Q18"/>
-      <c r="R18"/>
+      <c r="R18" s="42"/>
       <c r="S18"/>
       <c r="T18"/>
       <c r="U18"/>
@@ -54467,15 +54203,19 @@
         <v>3</v>
       </c>
       <c r="M19" s="42">
+        <v>4.0555555555555554</v>
+      </c>
+      <c r="N19" s="42">
         <v>2.9764011799410031</v>
       </c>
-      <c r="N19" s="42"/>
-      <c r="O19" s="42">
+      <c r="O19" s="42"/>
+      <c r="P19" s="42">
+        <v>7.6571428571428575</v>
+      </c>
+      <c r="Q19" s="42">
         <v>7.1635220125786168</v>
       </c>
-      <c r="P19" s="42"/>
-      <c r="Q19"/>
-      <c r="R19"/>
+      <c r="R19" s="42"/>
       <c r="S19"/>
       <c r="T19"/>
       <c r="U19"/>
@@ -54528,19 +54268,23 @@
         <v>4</v>
       </c>
       <c r="M20" s="42">
+        <v>4.166666666666667</v>
+      </c>
+      <c r="N20" s="42">
         <v>2.8849557522123894</v>
       </c>
-      <c r="N20" s="42">
+      <c r="O20" s="42">
         <v>0.17699115044247787</v>
       </c>
-      <c r="O20" s="42">
+      <c r="P20" s="42">
+        <v>7.409523809523809</v>
+      </c>
+      <c r="Q20" s="42">
         <v>7.5723270440251573</v>
       </c>
-      <c r="P20" s="42">
+      <c r="R20" s="42">
         <v>0.12641509433962261</v>
       </c>
-      <c r="Q20"/>
-      <c r="R20"/>
       <c r="S20"/>
       <c r="T20"/>
       <c r="U20"/>
@@ -54590,14 +54334,14 @@
       </c>
       <c r="K21"/>
       <c r="L21" s="23" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="M21" s="42"/>
       <c r="N21" s="42"/>
       <c r="O21" s="42"/>
       <c r="P21" s="42"/>
-      <c r="Q21"/>
-      <c r="R21"/>
+      <c r="Q21" s="42"/>
+      <c r="R21" s="42"/>
       <c r="S21"/>
       <c r="T21"/>
       <c r="U21"/>
@@ -54650,15 +54394,19 @@
         <v>1</v>
       </c>
       <c r="M22" s="42">
+        <v>1.7222222222222223</v>
+      </c>
+      <c r="N22" s="42">
         <v>0.98230088495575218</v>
       </c>
-      <c r="N22" s="42"/>
-      <c r="O22" s="42">
+      <c r="O22" s="42"/>
+      <c r="P22" s="42">
+        <v>3.2857142857142856</v>
+      </c>
+      <c r="Q22" s="42">
         <v>1.4968553459119498</v>
       </c>
-      <c r="P22" s="42"/>
-      <c r="Q22"/>
-      <c r="R22"/>
+      <c r="R22" s="42"/>
       <c r="S22"/>
       <c r="T22"/>
       <c r="U22"/>
@@ -54711,15 +54459,19 @@
         <v>2</v>
       </c>
       <c r="M23" s="42">
+        <v>2.7222222222222223</v>
+      </c>
+      <c r="N23" s="42">
         <v>1.4926253687315636</v>
       </c>
-      <c r="N23" s="42"/>
-      <c r="O23" s="42">
+      <c r="O23" s="42"/>
+      <c r="P23" s="42">
+        <v>5.8380952380952378</v>
+      </c>
+      <c r="Q23" s="42">
         <v>2.5786163522012577</v>
       </c>
-      <c r="P23" s="42"/>
-      <c r="Q23"/>
-      <c r="R23"/>
+      <c r="R23" s="42"/>
       <c r="S23"/>
       <c r="T23"/>
       <c r="U23"/>
@@ -54772,15 +54524,19 @@
         <v>3</v>
       </c>
       <c r="M24" s="42">
+        <v>2.9166666666666665</v>
+      </c>
+      <c r="N24" s="42">
         <v>1.5250737463126844</v>
       </c>
-      <c r="N24" s="42"/>
-      <c r="O24" s="42">
+      <c r="O24" s="42"/>
+      <c r="P24" s="42">
+        <v>7.1380952380952385</v>
+      </c>
+      <c r="Q24" s="42">
         <v>3.1069182389937104</v>
       </c>
-      <c r="P24" s="42"/>
-      <c r="Q24"/>
-      <c r="R24"/>
+      <c r="R24" s="42"/>
       <c r="S24"/>
       <c r="T24"/>
       <c r="U24"/>
@@ -54833,19 +54589,23 @@
         <v>4</v>
       </c>
       <c r="M25" s="42">
+        <v>3.1111111111111112</v>
+      </c>
+      <c r="N25" s="42">
         <v>1.5309734513274336</v>
       </c>
-      <c r="N25" s="42">
+      <c r="O25" s="42">
         <v>0.17699115044247787</v>
       </c>
-      <c r="O25" s="42">
+      <c r="P25" s="42">
+        <v>7.8571428571428568</v>
+      </c>
+      <c r="Q25" s="42">
         <v>3.4528301886792452</v>
       </c>
-      <c r="P25" s="42">
+      <c r="R25" s="42">
         <v>0.13962264150943396</v>
       </c>
-      <c r="Q25"/>
-      <c r="R25"/>
       <c r="S25"/>
       <c r="T25"/>
       <c r="U25"/>
@@ -55853,11 +55613,11 @@
         <v>11</v>
       </c>
       <c r="H50" s="11">
-        <v>33.9</v>
+        <v>36</v>
       </c>
       <c r="I50" s="11">
         <f>G50/H50</f>
-        <v>0.32448377581120946</v>
+        <v>0.30555555555555558</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
@@ -60154,56 +59914,56 @@
       <c r="A194" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B194" s="11" t="s">
+      <c r="B194" t="s">
         <v>33</v>
       </c>
-      <c r="C194" s="29">
+      <c r="C194">
         <v>26</v>
       </c>
-      <c r="D194" s="29">
-        <v>1</v>
-      </c>
-      <c r="E194" s="29">
+      <c r="D194">
+        <v>1</v>
+      </c>
+      <c r="E194">
         <v>1</v>
       </c>
       <c r="F194">
-        <v>1.95</v>
+        <v>1.19</v>
       </c>
       <c r="G194">
-        <v>5.2</v>
+        <v>14.1</v>
       </c>
       <c r="H194" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I194" s="11">
         <f>G194/H194</f>
-        <v>0.37142857142857144</v>
+        <v>0.67142857142857137</v>
       </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A195" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B195" s="11" t="s">
+      <c r="B195" t="s">
         <v>34</v>
       </c>
-      <c r="C195" s="29">
+      <c r="C195">
         <v>26</v>
       </c>
-      <c r="D195" s="29">
-        <v>1</v>
-      </c>
-      <c r="E195" s="29">
+      <c r="D195">
+        <v>1</v>
+      </c>
+      <c r="E195">
         <v>1</v>
       </c>
       <c r="F195">
-        <v>1.95</v>
+        <v>1.18</v>
       </c>
       <c r="G195">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H195" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I195" s="11">
         <f t="shared" ref="I195:I205" si="13">G195/H195</f>
@@ -60214,1380 +59974,1380 @@
       <c r="A196" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B196" s="11" t="s">
+      <c r="B196" t="s">
         <v>35</v>
       </c>
-      <c r="C196" s="29">
+      <c r="C196">
         <v>26</v>
       </c>
-      <c r="D196" s="29">
-        <v>1</v>
-      </c>
-      <c r="E196" s="29">
+      <c r="D196">
+        <v>1</v>
+      </c>
+      <c r="E196">
         <v>1</v>
       </c>
       <c r="F196">
-        <v>1.95</v>
+        <v>1.18</v>
       </c>
       <c r="G196">
-        <v>16.399999999999999</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="H196" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I196" s="11">
         <f t="shared" si="13"/>
-        <v>1.1714285714285713</v>
+        <v>0.93333333333333335</v>
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A197" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B197" s="11" t="s">
+      <c r="B197" t="s">
         <v>33</v>
       </c>
-      <c r="C197" s="29">
+      <c r="C197">
         <v>26</v>
       </c>
-      <c r="D197" s="29">
+      <c r="D197">
         <v>2</v>
       </c>
-      <c r="E197" s="29">
+      <c r="E197">
         <v>1</v>
       </c>
       <c r="F197">
-        <v>1.95</v>
+        <v>1.19</v>
       </c>
       <c r="G197">
-        <v>9.1999999999999993</v>
+        <v>27.1</v>
       </c>
       <c r="H197" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I197" s="11">
         <f t="shared" si="13"/>
-        <v>0.65714285714285714</v>
+        <v>1.2904761904761906</v>
       </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A198" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B198" s="11" t="s">
+      <c r="B198" t="s">
         <v>34</v>
       </c>
-      <c r="C198" s="29">
+      <c r="C198">
         <v>26</v>
       </c>
-      <c r="D198" s="29">
+      <c r="D198">
         <v>2</v>
       </c>
-      <c r="E198" s="29">
+      <c r="E198">
         <v>1</v>
       </c>
       <c r="F198">
-        <v>1.95</v>
+        <v>1.18</v>
       </c>
       <c r="G198">
-        <v>21.1</v>
+        <v>34.4</v>
       </c>
       <c r="H198" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I198" s="11">
         <f t="shared" si="13"/>
-        <v>1.5071428571428573</v>
+        <v>1.638095238095238</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A199" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B199" s="11" t="s">
+      <c r="B199" t="s">
         <v>35</v>
       </c>
-      <c r="C199" s="29">
+      <c r="C199">
         <v>26</v>
       </c>
-      <c r="D199" s="29">
+      <c r="D199">
         <v>2</v>
       </c>
-      <c r="E199" s="29">
+      <c r="E199">
         <v>1</v>
       </c>
       <c r="F199">
-        <v>1.95</v>
+        <v>1.19</v>
       </c>
       <c r="G199">
-        <v>28.5</v>
+        <v>33.5</v>
       </c>
       <c r="H199" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I199" s="11">
         <f t="shared" si="13"/>
-        <v>2.0357142857142856</v>
+        <v>1.5952380952380953</v>
       </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A200" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B200" s="11" t="s">
+      <c r="B200" t="s">
         <v>33</v>
       </c>
-      <c r="C200" s="29">
+      <c r="C200">
         <v>26</v>
       </c>
-      <c r="D200" s="29">
-        <v>3</v>
-      </c>
-      <c r="E200" s="29">
+      <c r="D200">
+        <v>3</v>
+      </c>
+      <c r="E200">
         <v>1</v>
       </c>
       <c r="F200">
-        <v>1.95</v>
+        <v>1.18</v>
       </c>
       <c r="G200">
-        <v>10.3</v>
+        <v>23.5</v>
       </c>
       <c r="H200" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I200" s="11">
         <f t="shared" si="13"/>
-        <v>0.73571428571428577</v>
+        <v>1.1190476190476191</v>
       </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A201" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B201" s="11" t="s">
+      <c r="B201" t="s">
         <v>34</v>
       </c>
-      <c r="C201" s="29">
+      <c r="C201">
         <v>26</v>
       </c>
-      <c r="D201" s="29">
-        <v>3</v>
-      </c>
-      <c r="E201" s="29">
+      <c r="D201">
+        <v>3</v>
+      </c>
+      <c r="E201">
         <v>1</v>
       </c>
       <c r="F201">
-        <v>1.95</v>
+        <v>1.18</v>
       </c>
       <c r="G201">
-        <v>32.5</v>
+        <v>34.9</v>
       </c>
       <c r="H201" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I201" s="11">
         <f t="shared" si="13"/>
-        <v>2.3214285714285716</v>
+        <v>1.6619047619047618</v>
       </c>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A202" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B202" s="11" t="s">
+      <c r="B202" t="s">
         <v>35</v>
       </c>
-      <c r="C202" s="29">
+      <c r="C202">
         <v>26</v>
       </c>
-      <c r="D202" s="29">
-        <v>3</v>
-      </c>
-      <c r="E202" s="29">
+      <c r="D202">
+        <v>3</v>
+      </c>
+      <c r="E202">
         <v>1</v>
       </c>
       <c r="F202">
-        <v>1.95</v>
+        <v>1.18</v>
       </c>
       <c r="G202">
-        <v>34.200000000000003</v>
+        <v>34.5</v>
       </c>
       <c r="H202" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I202" s="11">
         <f t="shared" si="13"/>
-        <v>2.4428571428571431</v>
+        <v>1.6428571428571428</v>
       </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A203" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B203" s="11" t="s">
+      <c r="B203" t="s">
         <v>33</v>
       </c>
-      <c r="C203" s="29">
+      <c r="C203">
         <v>26</v>
       </c>
-      <c r="D203" s="29">
+      <c r="D203">
         <v>4</v>
       </c>
-      <c r="E203" s="29">
+      <c r="E203">
         <v>1</v>
       </c>
       <c r="F203">
-        <v>1.95</v>
+        <v>1.18</v>
       </c>
       <c r="G203">
-        <v>13.3</v>
+        <v>31.4</v>
       </c>
       <c r="H203" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I203" s="11">
         <f t="shared" si="13"/>
-        <v>0.95000000000000007</v>
+        <v>1.4952380952380953</v>
       </c>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A204" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B204" s="11" t="s">
+      <c r="B204" t="s">
         <v>34</v>
       </c>
-      <c r="C204" s="29">
+      <c r="C204">
         <v>26</v>
       </c>
-      <c r="D204" s="29">
+      <c r="D204">
         <v>4</v>
       </c>
-      <c r="E204" s="29">
+      <c r="E204">
         <v>1</v>
       </c>
       <c r="F204">
-        <v>1.95</v>
+        <v>1.19</v>
       </c>
       <c r="G204">
-        <v>37.200000000000003</v>
+        <v>37.9</v>
       </c>
       <c r="H204" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I204" s="11">
         <f t="shared" si="13"/>
-        <v>2.6571428571428575</v>
+        <v>1.8047619047619048</v>
       </c>
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A205" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B205" s="11" t="s">
+      <c r="B205" t="s">
         <v>35</v>
       </c>
-      <c r="C205" s="29">
+      <c r="C205">
         <v>26</v>
       </c>
-      <c r="D205" s="29">
+      <c r="D205">
         <v>4</v>
       </c>
-      <c r="E205" s="29">
+      <c r="E205">
         <v>1</v>
       </c>
       <c r="F205">
-        <v>1.95</v>
+        <v>1.19</v>
       </c>
       <c r="G205">
-        <v>37.200000000000003</v>
+        <v>36.9</v>
       </c>
       <c r="H205" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I205" s="11">
         <f t="shared" si="13"/>
-        <v>2.6571428571428575</v>
+        <v>1.7571428571428571</v>
       </c>
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A206" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B206" s="11" t="s">
+      <c r="B206" t="s">
         <v>33</v>
       </c>
-      <c r="C206" s="29">
+      <c r="C206">
         <v>26</v>
       </c>
-      <c r="D206" s="29">
-        <v>1</v>
-      </c>
-      <c r="E206" s="29">
+      <c r="D206">
+        <v>1</v>
+      </c>
+      <c r="E206">
         <v>2</v>
       </c>
       <c r="F206">
-        <v>1.88</v>
+        <v>6.2</v>
       </c>
       <c r="G206">
-        <v>19.8</v>
+        <v>45.3</v>
       </c>
       <c r="H206" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I206" s="11">
         <f>G206/H206</f>
-        <v>1.4142857142857144</v>
+        <v>2.157142857142857</v>
       </c>
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A207" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B207" s="11" t="s">
+      <c r="B207" t="s">
         <v>34</v>
       </c>
-      <c r="C207" s="29">
+      <c r="C207">
         <v>26</v>
       </c>
-      <c r="D207" s="29">
-        <v>1</v>
-      </c>
-      <c r="E207" s="29">
+      <c r="D207">
+        <v>1</v>
+      </c>
+      <c r="E207">
         <v>2</v>
       </c>
       <c r="F207">
-        <v>1.89</v>
+        <v>6.2</v>
       </c>
       <c r="G207">
-        <v>65.900000000000006</v>
+        <v>76.8</v>
       </c>
       <c r="H207" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I207" s="11">
         <f t="shared" ref="I207:I217" si="14">G207/H207</f>
-        <v>4.7071428571428573</v>
+        <v>3.657142857142857</v>
       </c>
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A208" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B208" s="11" t="s">
+      <c r="B208" t="s">
         <v>35</v>
       </c>
-      <c r="C208" s="29">
+      <c r="C208">
         <v>26</v>
       </c>
-      <c r="D208" s="29">
-        <v>1</v>
-      </c>
-      <c r="E208" s="29">
+      <c r="D208">
+        <v>1</v>
+      </c>
+      <c r="E208">
         <v>2</v>
       </c>
       <c r="F208">
-        <v>1.89</v>
+        <v>6.2</v>
       </c>
       <c r="G208">
-        <v>66.2</v>
+        <v>75.7</v>
       </c>
       <c r="H208" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I208" s="11">
         <f t="shared" si="14"/>
-        <v>4.7285714285714286</v>
+        <v>3.6047619047619048</v>
       </c>
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A209" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B209" s="11" t="s">
+      <c r="B209" t="s">
         <v>33</v>
       </c>
-      <c r="C209" s="29">
+      <c r="C209">
         <v>26</v>
       </c>
-      <c r="D209" s="29">
+      <c r="D209">
         <v>2</v>
       </c>
-      <c r="E209" s="29">
+      <c r="E209">
         <v>2</v>
       </c>
       <c r="F209">
-        <v>1.89</v>
+        <v>6.21</v>
       </c>
       <c r="G209">
-        <v>35.6</v>
+        <v>83.7</v>
       </c>
       <c r="H209" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I209" s="11">
         <f t="shared" si="14"/>
-        <v>2.5428571428571431</v>
+        <v>3.9857142857142858</v>
       </c>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A210" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B210" s="11" t="s">
+      <c r="B210" t="s">
         <v>34</v>
       </c>
-      <c r="C210" s="29">
+      <c r="C210">
         <v>26</v>
       </c>
-      <c r="D210" s="29">
+      <c r="D210">
         <v>2</v>
       </c>
-      <c r="E210" s="29">
+      <c r="E210">
         <v>2</v>
       </c>
       <c r="F210">
-        <v>1.89</v>
+        <v>6.2</v>
       </c>
       <c r="G210">
-        <v>112.5</v>
+        <v>130.30000000000001</v>
       </c>
       <c r="H210" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I210" s="11">
         <f t="shared" si="14"/>
-        <v>8.0357142857142865</v>
+        <v>6.2047619047619049</v>
       </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A211" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B211" s="11" t="s">
+      <c r="B211" t="s">
         <v>35</v>
       </c>
-      <c r="C211" s="29">
+      <c r="C211">
         <v>26</v>
       </c>
-      <c r="D211" s="29">
+      <c r="D211">
         <v>2</v>
       </c>
-      <c r="E211" s="29">
+      <c r="E211">
         <v>2</v>
       </c>
       <c r="F211">
-        <v>1.89</v>
+        <v>6.2</v>
       </c>
       <c r="G211">
-        <v>127.6</v>
+        <v>140.4</v>
       </c>
       <c r="H211" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I211" s="11">
         <f t="shared" si="14"/>
-        <v>9.1142857142857139</v>
+        <v>6.6857142857142859</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A212" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B212" s="11" t="s">
+      <c r="B212" t="s">
         <v>33</v>
       </c>
-      <c r="C212" s="29">
+      <c r="C212">
         <v>26</v>
       </c>
-      <c r="D212" s="29">
-        <v>3</v>
-      </c>
-      <c r="E212" s="29">
+      <c r="D212">
+        <v>3</v>
+      </c>
+      <c r="E212">
         <v>2</v>
       </c>
       <c r="F212">
-        <v>1.89</v>
+        <v>6.21</v>
       </c>
       <c r="G212">
-        <v>48.6</v>
+        <v>112.7</v>
       </c>
       <c r="H212" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I212" s="11">
         <f t="shared" si="14"/>
-        <v>3.4714285714285715</v>
+        <v>5.3666666666666671</v>
       </c>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A213" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B213" s="11" t="s">
+      <c r="B213" t="s">
         <v>34</v>
       </c>
-      <c r="C213" s="29">
+      <c r="C213">
         <v>26</v>
       </c>
-      <c r="D213" s="29">
-        <v>3</v>
-      </c>
-      <c r="E213" s="29">
+      <c r="D213">
+        <v>3</v>
+      </c>
+      <c r="E213">
         <v>2</v>
       </c>
       <c r="F213">
-        <v>1.89</v>
+        <v>6.2</v>
       </c>
       <c r="G213">
-        <v>134.5</v>
+        <v>163.80000000000001</v>
       </c>
       <c r="H213" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I213" s="11">
         <f t="shared" si="14"/>
-        <v>9.6071428571428577</v>
+        <v>7.8000000000000007</v>
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A214" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B214" s="11" t="s">
+      <c r="B214" t="s">
         <v>35</v>
       </c>
-      <c r="C214" s="29">
+      <c r="C214">
         <v>26</v>
       </c>
-      <c r="D214" s="29">
-        <v>3</v>
-      </c>
-      <c r="E214" s="29">
+      <c r="D214">
+        <v>3</v>
+      </c>
+      <c r="E214">
         <v>2</v>
       </c>
       <c r="F214">
-        <v>1.89</v>
+        <v>6.2</v>
       </c>
       <c r="G214">
-        <v>114.5</v>
+        <v>146.19999999999999</v>
       </c>
       <c r="H214" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I214" s="11">
         <f t="shared" si="14"/>
-        <v>8.1785714285714288</v>
+        <v>6.9619047619047612</v>
       </c>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A215" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B215" s="11" t="s">
+      <c r="B215" t="s">
         <v>33</v>
       </c>
-      <c r="C215" s="29">
+      <c r="C215">
         <v>26</v>
       </c>
-      <c r="D215" s="29">
+      <c r="D215">
         <v>4</v>
       </c>
-      <c r="E215" s="29">
+      <c r="E215">
         <v>2</v>
       </c>
       <c r="F215">
-        <v>1.89</v>
+        <v>6.2</v>
       </c>
       <c r="G215">
-        <v>35.5</v>
+        <v>104.7</v>
       </c>
       <c r="H215" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I215" s="11">
         <f t="shared" si="14"/>
-        <v>2.5357142857142856</v>
+        <v>4.9857142857142858</v>
       </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A216" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B216" s="11" t="s">
+      <c r="B216" t="s">
         <v>34</v>
       </c>
-      <c r="C216" s="29">
+      <c r="C216">
         <v>26</v>
       </c>
-      <c r="D216" s="29">
+      <c r="D216">
         <v>4</v>
       </c>
-      <c r="E216" s="29">
+      <c r="E216">
         <v>2</v>
       </c>
       <c r="F216">
-        <v>1.89</v>
+        <v>6.2</v>
       </c>
       <c r="G216">
-        <v>120.2</v>
+        <v>165.3</v>
       </c>
       <c r="H216" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I216" s="11">
         <f t="shared" si="14"/>
-        <v>8.5857142857142854</v>
+        <v>7.8714285714285719</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A217" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B217" s="11" t="s">
+      <c r="B217" t="s">
         <v>35</v>
       </c>
-      <c r="C217" s="29">
+      <c r="C217">
         <v>26</v>
       </c>
-      <c r="D217" s="29">
+      <c r="D217">
         <v>4</v>
       </c>
-      <c r="E217" s="29">
+      <c r="E217">
         <v>2</v>
       </c>
       <c r="F217">
-        <v>1.89</v>
+        <v>6.2</v>
       </c>
       <c r="G217">
-        <v>150.1</v>
+        <v>149.69999999999999</v>
       </c>
       <c r="H217" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I217" s="11">
         <f t="shared" si="14"/>
-        <v>10.721428571428572</v>
+        <v>7.1285714285714281</v>
       </c>
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A218" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B218" s="11" t="s">
+      <c r="B218" t="s">
         <v>33</v>
       </c>
-      <c r="C218" s="29">
+      <c r="C218">
         <v>26</v>
       </c>
-      <c r="D218" s="29">
-        <v>1</v>
-      </c>
-      <c r="E218" s="29">
+      <c r="D218">
+        <v>1</v>
+      </c>
+      <c r="E218">
         <v>3</v>
       </c>
       <c r="F218">
-        <v>3</v>
+        <v>12.04</v>
       </c>
       <c r="G218">
-        <v>6.2</v>
+        <v>14.6</v>
       </c>
       <c r="H218" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I218" s="11">
         <f>G218/H218</f>
-        <v>0.44285714285714289</v>
+        <v>0.69523809523809521</v>
       </c>
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A219" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B219" s="11" t="s">
+      <c r="B219" t="s">
         <v>34</v>
       </c>
-      <c r="C219" s="29">
+      <c r="C219">
         <v>26</v>
       </c>
-      <c r="D219" s="29">
-        <v>1</v>
-      </c>
-      <c r="E219" s="29">
+      <c r="D219">
+        <v>1</v>
+      </c>
+      <c r="E219">
         <v>3</v>
       </c>
       <c r="F219">
-        <v>3</v>
+        <v>11.93</v>
       </c>
       <c r="G219">
-        <v>46.9</v>
+        <v>67</v>
       </c>
       <c r="H219" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I219" s="11">
         <f t="shared" ref="I219:I229" si="15">G219/H219</f>
-        <v>3.35</v>
+        <v>3.1904761904761907</v>
       </c>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A220" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B220" s="11" t="s">
+      <c r="B220" t="s">
         <v>35</v>
       </c>
-      <c r="C220" s="29">
+      <c r="C220">
         <v>26</v>
       </c>
-      <c r="D220" s="29">
-        <v>1</v>
-      </c>
-      <c r="E220" s="29">
+      <c r="D220">
+        <v>1</v>
+      </c>
+      <c r="E220">
         <v>3</v>
       </c>
       <c r="F220">
-        <v>3</v>
+        <v>11.94</v>
       </c>
       <c r="G220">
-        <v>50.8</v>
+        <v>73.5</v>
       </c>
       <c r="H220" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I220" s="11">
         <f t="shared" si="15"/>
-        <v>3.6285714285714286</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A221" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B221" s="11" t="s">
+      <c r="B221" t="s">
         <v>33</v>
       </c>
-      <c r="C221" s="29">
+      <c r="C221">
         <v>26</v>
       </c>
-      <c r="D221" s="29">
+      <c r="D221">
         <v>2</v>
       </c>
-      <c r="E221" s="29">
+      <c r="E221">
         <v>3</v>
       </c>
       <c r="F221">
-        <v>3</v>
+        <v>11.95</v>
       </c>
       <c r="G221">
-        <v>11</v>
+        <v>32.5</v>
       </c>
       <c r="H221" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I221" s="11">
         <f t="shared" si="15"/>
-        <v>0.7857142857142857</v>
+        <v>1.5476190476190477</v>
       </c>
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A222" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B222" s="11" t="s">
+      <c r="B222" t="s">
         <v>34</v>
       </c>
-      <c r="C222" s="29">
+      <c r="C222">
         <v>26</v>
       </c>
-      <c r="D222" s="29">
+      <c r="D222">
         <v>2</v>
       </c>
-      <c r="E222" s="29">
+      <c r="E222">
         <v>3</v>
       </c>
       <c r="F222">
-        <v>3</v>
+        <v>11.93</v>
       </c>
       <c r="G222">
-        <v>101.2</v>
+        <v>131.69999999999999</v>
       </c>
       <c r="H222" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I222" s="11">
         <f t="shared" si="15"/>
-        <v>7.2285714285714286</v>
+        <v>6.2714285714285705</v>
       </c>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A223" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B223" s="11" t="s">
+      <c r="B223" t="s">
         <v>35</v>
       </c>
-      <c r="C223" s="29">
+      <c r="C223">
         <v>26</v>
       </c>
-      <c r="D223" s="29">
+      <c r="D223">
         <v>2</v>
       </c>
-      <c r="E223" s="29">
+      <c r="E223">
         <v>3</v>
       </c>
       <c r="F223">
-        <v>3</v>
+        <v>11.93</v>
       </c>
       <c r="G223">
-        <v>79.5</v>
+        <v>132.19999999999999</v>
       </c>
       <c r="H223" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I223" s="11">
         <f t="shared" si="15"/>
-        <v>5.6785714285714288</v>
+        <v>6.2952380952380951</v>
       </c>
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A224" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B224" s="11" t="s">
+      <c r="B224" t="s">
         <v>33</v>
       </c>
-      <c r="C224" s="29">
+      <c r="C224">
         <v>26</v>
       </c>
-      <c r="D224" s="29">
-        <v>3</v>
-      </c>
-      <c r="E224" s="29">
+      <c r="D224">
+        <v>3</v>
+      </c>
+      <c r="E224">
         <v>3</v>
       </c>
       <c r="F224">
-        <v>3</v>
+        <v>11.96</v>
       </c>
       <c r="G224">
-        <v>18.399999999999999</v>
+        <v>42.3</v>
       </c>
       <c r="H224" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I224" s="11">
         <f t="shared" si="15"/>
-        <v>1.3142857142857143</v>
+        <v>2.0142857142857142</v>
       </c>
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A225" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B225" s="11" t="s">
+      <c r="B225" t="s">
         <v>34</v>
       </c>
-      <c r="C225" s="29">
+      <c r="C225">
         <v>26</v>
       </c>
-      <c r="D225" s="29">
-        <v>3</v>
-      </c>
-      <c r="E225" s="29">
+      <c r="D225">
+        <v>3</v>
+      </c>
+      <c r="E225">
         <v>3</v>
       </c>
       <c r="F225">
-        <v>3</v>
+        <v>11.93</v>
       </c>
       <c r="G225">
-        <v>109</v>
+        <v>154.80000000000001</v>
       </c>
       <c r="H225" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I225" s="11">
         <f t="shared" si="15"/>
-        <v>7.7857142857142856</v>
+        <v>7.3714285714285719</v>
       </c>
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A226" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B226" s="11" t="s">
+      <c r="B226" t="s">
         <v>35</v>
       </c>
-      <c r="C226" s="29">
+      <c r="C226">
         <v>26</v>
       </c>
-      <c r="D226" s="29">
-        <v>3</v>
-      </c>
-      <c r="E226" s="29">
+      <c r="D226">
+        <v>3</v>
+      </c>
+      <c r="E226">
         <v>3</v>
       </c>
       <c r="F226">
-        <v>3</v>
+        <v>11.93</v>
       </c>
       <c r="G226">
-        <v>100.5</v>
+        <v>160.80000000000001</v>
       </c>
       <c r="H226" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I226" s="11">
         <f t="shared" si="15"/>
-        <v>7.1785714285714288</v>
+        <v>7.6571428571428575</v>
       </c>
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A227" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B227" s="11" t="s">
+      <c r="B227" t="s">
         <v>33</v>
       </c>
-      <c r="C227" s="29">
+      <c r="C227">
         <v>26</v>
       </c>
-      <c r="D227" s="29">
+      <c r="D227">
         <v>4</v>
       </c>
-      <c r="E227" s="29">
+      <c r="E227">
         <v>3</v>
       </c>
       <c r="F227">
-        <v>3</v>
+        <v>11.96</v>
       </c>
       <c r="G227">
-        <v>20.3</v>
+        <v>47.6</v>
       </c>
       <c r="H227" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I227" s="11">
         <f t="shared" si="15"/>
-        <v>1.45</v>
+        <v>2.2666666666666666</v>
       </c>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A228" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B228" s="11" t="s">
+      <c r="B228" t="s">
         <v>34</v>
       </c>
-      <c r="C228" s="29">
+      <c r="C228">
         <v>26</v>
       </c>
-      <c r="D228" s="29">
+      <c r="D228">
         <v>4</v>
       </c>
-      <c r="E228" s="29">
+      <c r="E228">
         <v>3</v>
       </c>
       <c r="F228">
-        <v>3</v>
+        <v>11.93</v>
       </c>
       <c r="G228">
-        <v>112.4</v>
+        <v>168.1</v>
       </c>
       <c r="H228" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I228" s="11">
         <f t="shared" si="15"/>
-        <v>8.0285714285714285</v>
+        <v>8.0047619047619047</v>
       </c>
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A229" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B229" s="11" t="s">
+      <c r="B229" t="s">
         <v>35</v>
       </c>
-      <c r="C229" s="29">
+      <c r="C229">
         <v>26</v>
       </c>
-      <c r="D229" s="29">
+      <c r="D229">
         <v>4</v>
       </c>
-      <c r="E229" s="29">
+      <c r="E229">
         <v>3</v>
       </c>
       <c r="F229">
-        <v>3</v>
+        <v>11.93</v>
       </c>
       <c r="G229">
-        <v>111.6</v>
+        <v>155.6</v>
       </c>
       <c r="H229" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I229" s="11">
         <f t="shared" si="15"/>
-        <v>7.9714285714285706</v>
+        <v>7.409523809523809</v>
       </c>
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A230" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B230" s="11" t="s">
+      <c r="B230" t="s">
         <v>33</v>
       </c>
-      <c r="C230" s="29">
+      <c r="C230">
         <v>26</v>
       </c>
-      <c r="D230" s="29">
-        <v>1</v>
-      </c>
-      <c r="E230" s="29">
+      <c r="D230">
+        <v>1</v>
+      </c>
+      <c r="E230">
         <v>4</v>
       </c>
       <c r="F230">
-        <v>3.86</v>
+        <v>18.260000000000002</v>
       </c>
       <c r="G230">
-        <v>5.2</v>
+        <v>10.6</v>
       </c>
       <c r="H230" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I230" s="11">
         <f>G230/H230</f>
-        <v>0.37142857142857144</v>
+        <v>0.50476190476190474</v>
       </c>
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A231" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B231" s="11" t="s">
+      <c r="B231" t="s">
         <v>34</v>
       </c>
-      <c r="C231" s="29">
+      <c r="C231">
         <v>26</v>
       </c>
-      <c r="D231" s="29">
-        <v>1</v>
-      </c>
-      <c r="E231" s="29">
+      <c r="D231">
+        <v>1</v>
+      </c>
+      <c r="E231">
         <v>4</v>
       </c>
       <c r="F231">
-        <v>3.86</v>
+        <v>18.239999999999998</v>
       </c>
       <c r="G231">
-        <v>54.3</v>
+        <v>70.099999999999994</v>
       </c>
       <c r="H231" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I231" s="11">
         <f t="shared" ref="I231:I293" si="16">G231/H231</f>
-        <v>3.8785714285714286</v>
+        <v>3.3380952380952378</v>
       </c>
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A232" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B232" s="11" t="s">
+      <c r="B232" t="s">
         <v>35</v>
       </c>
-      <c r="C232" s="29">
+      <c r="C232">
         <v>26</v>
       </c>
-      <c r="D232" s="29">
-        <v>1</v>
-      </c>
-      <c r="E232" s="29">
+      <c r="D232">
+        <v>1</v>
+      </c>
+      <c r="E232">
         <v>4</v>
       </c>
       <c r="F232">
-        <v>3.85</v>
+        <v>18.23</v>
       </c>
       <c r="G232">
-        <v>55.1</v>
+        <v>69</v>
       </c>
       <c r="H232" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I232" s="11">
         <f t="shared" si="16"/>
-        <v>3.9357142857142859</v>
+        <v>3.2857142857142856</v>
       </c>
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A233" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B233" s="11" t="s">
+      <c r="B233" t="s">
         <v>33</v>
       </c>
-      <c r="C233" s="29">
+      <c r="C233">
         <v>26</v>
       </c>
-      <c r="D233" s="29">
+      <c r="D233">
         <v>2</v>
       </c>
-      <c r="E233" s="29">
+      <c r="E233">
         <v>4</v>
       </c>
       <c r="F233">
-        <v>3.85</v>
+        <v>18.260000000000002</v>
       </c>
       <c r="G233">
-        <v>5.9</v>
+        <v>21.1</v>
       </c>
       <c r="H233" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I233" s="11">
         <f t="shared" si="16"/>
-        <v>0.42142857142857143</v>
+        <v>1.0047619047619047</v>
       </c>
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A234" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B234" s="11" t="s">
+      <c r="B234" t="s">
         <v>34</v>
       </c>
-      <c r="C234" s="29">
+      <c r="C234">
         <v>26</v>
       </c>
-      <c r="D234" s="29">
+      <c r="D234">
         <v>2</v>
       </c>
-      <c r="E234" s="29">
+      <c r="E234">
         <v>4</v>
       </c>
       <c r="F234">
-        <v>3.86</v>
+        <v>18.239999999999998</v>
       </c>
       <c r="G234">
-        <v>103.5</v>
+        <v>129.4</v>
       </c>
       <c r="H234" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I234" s="11">
         <f t="shared" si="16"/>
-        <v>7.3928571428571432</v>
+        <v>6.1619047619047622</v>
       </c>
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A235" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B235" s="11" t="s">
+      <c r="B235" t="s">
         <v>35</v>
       </c>
-      <c r="C235" s="29">
+      <c r="C235">
         <v>26</v>
       </c>
-      <c r="D235" s="29">
+      <c r="D235">
         <v>2</v>
       </c>
-      <c r="E235" s="29">
+      <c r="E235">
         <v>4</v>
       </c>
       <c r="F235">
-        <v>3.86</v>
+        <v>18.23</v>
       </c>
       <c r="G235">
-        <v>104.5</v>
+        <v>122.6</v>
       </c>
       <c r="H235" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I235" s="11">
         <f t="shared" si="16"/>
-        <v>7.4642857142857144</v>
+        <v>5.8380952380952378</v>
       </c>
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A236" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B236" s="11" t="s">
+      <c r="B236" t="s">
         <v>33</v>
       </c>
-      <c r="C236" s="29">
+      <c r="C236">
         <v>26</v>
       </c>
-      <c r="D236" s="29">
-        <v>3</v>
-      </c>
-      <c r="E236" s="29">
+      <c r="D236">
+        <v>3</v>
+      </c>
+      <c r="E236">
         <v>4</v>
       </c>
       <c r="F236">
-        <v>3.84</v>
+        <v>18.25</v>
       </c>
       <c r="G236">
-        <v>11</v>
+        <v>26.2</v>
       </c>
       <c r="H236" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I236" s="11">
         <f t="shared" si="16"/>
-        <v>0.7857142857142857</v>
+        <v>1.2476190476190476</v>
       </c>
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A237" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B237" s="11" t="s">
+      <c r="B237" t="s">
         <v>34</v>
       </c>
-      <c r="C237" s="29">
+      <c r="C237">
         <v>26</v>
       </c>
-      <c r="D237" s="29">
-        <v>3</v>
-      </c>
-      <c r="E237" s="29">
+      <c r="D237">
+        <v>3</v>
+      </c>
+      <c r="E237">
         <v>4</v>
       </c>
       <c r="F237">
-        <v>3.86</v>
+        <v>18.239999999999998</v>
       </c>
       <c r="G237">
-        <v>111</v>
+        <v>150.6</v>
       </c>
       <c r="H237" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I237" s="11">
         <f t="shared" si="16"/>
-        <v>7.9285714285714288</v>
+        <v>7.1714285714285708</v>
       </c>
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A238" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B238" s="11" t="s">
+      <c r="B238" t="s">
         <v>35</v>
       </c>
-      <c r="C238" s="29">
+      <c r="C238">
         <v>26</v>
       </c>
-      <c r="D238" s="29">
-        <v>3</v>
-      </c>
-      <c r="E238" s="29">
+      <c r="D238">
+        <v>3</v>
+      </c>
+      <c r="E238">
         <v>4</v>
       </c>
       <c r="F238">
-        <v>3.86</v>
+        <v>18.22</v>
       </c>
       <c r="G238">
-        <v>111.4</v>
+        <v>149.9</v>
       </c>
       <c r="H238" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I238" s="11">
         <f t="shared" si="16"/>
-        <v>7.9571428571428573</v>
+        <v>7.1380952380952385</v>
       </c>
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A239" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B239" s="11" t="s">
+      <c r="B239" t="s">
         <v>33</v>
       </c>
-      <c r="C239" s="29">
+      <c r="C239">
         <v>26</v>
       </c>
-      <c r="D239" s="29">
+      <c r="D239">
         <v>4</v>
       </c>
-      <c r="E239" s="29">
+      <c r="E239">
         <v>4</v>
       </c>
       <c r="F239">
-        <v>3.86</v>
+        <v>18.23</v>
       </c>
       <c r="G239">
-        <v>12.3</v>
+        <v>29.2</v>
       </c>
       <c r="H239" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I239" s="11">
         <f t="shared" si="16"/>
-        <v>0.87857142857142867</v>
+        <v>1.3904761904761904</v>
       </c>
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A240" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B240" s="11" t="s">
+      <c r="B240" t="s">
         <v>34</v>
       </c>
-      <c r="C240" s="29">
+      <c r="C240">
         <v>26</v>
       </c>
-      <c r="D240" s="29">
+      <c r="D240">
         <v>4</v>
       </c>
-      <c r="E240" s="29">
+      <c r="E240">
         <v>4</v>
       </c>
       <c r="F240">
-        <v>3.86</v>
+        <v>18.23</v>
       </c>
       <c r="G240">
-        <v>124.7</v>
+        <v>167.2</v>
       </c>
       <c r="H240" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I240" s="11">
         <f t="shared" si="16"/>
-        <v>8.9071428571428566</v>
+        <v>7.9619047619047612</v>
       </c>
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A241" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="B241" s="11" t="s">
+      <c r="B241" t="s">
         <v>35</v>
       </c>
-      <c r="C241" s="29">
+      <c r="C241">
         <v>26</v>
       </c>
-      <c r="D241" s="29">
+      <c r="D241">
         <v>4</v>
       </c>
-      <c r="E241" s="29">
+      <c r="E241">
         <v>4</v>
       </c>
       <c r="F241">
-        <v>3.86</v>
+        <v>18.23</v>
       </c>
       <c r="G241">
-        <v>123.9</v>
+        <v>165</v>
       </c>
       <c r="H241" s="11">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="I241" s="11">
         <f t="shared" si="16"/>
-        <v>8.85</v>
+        <v>7.8571428571428568</v>
       </c>
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.3">
@@ -63272,7 +63032,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting pivot="1" sqref="M6:P25">
+  <conditionalFormatting pivot="1" sqref="M6:R25">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>